<commit_message>
[FIX] - Catering Bintang
</commit_message>
<xml_diff>
--- a/resources/template/BINTANG.xlsx
+++ b/resources/template/BINTANG.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hallo_ppa\public\storage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hallo_ppa\resources\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9E8CAC-9497-472D-9E73-EB74A1723F16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFDF241-5F2B-4746-8464-EF642F1428D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{96DAB095-C63E-43E2-9BFC-56E2EB8E01C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="97">
   <si>
     <t>LOKASI</t>
   </si>
@@ -318,6 +318,9 @@
   </si>
   <si>
     <t>Mess Tambang A2</t>
+  </si>
+  <si>
+    <t>REBUSAN GL A2</t>
   </si>
 </sst>
 </file>
@@ -1173,10 +1176,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{727E0051-6F26-4AB8-8E1A-F7C7AFECA816}">
-  <dimension ref="A1:AK100"/>
+  <dimension ref="A1:AK101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="D91" sqref="A91:XFD91"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1378,7 +1381,7 @@
       <c r="AH3" s="10"/>
       <c r="AI3" s="10"/>
       <c r="AJ3" s="7">
-        <f t="shared" ref="AJ3:AJ37" si="0">SUM(E3:AI3)</f>
+        <f t="shared" ref="AJ3:AJ38" si="0">SUM(E3:AI3)</f>
         <v>0</v>
       </c>
       <c r="AK3" s="2"/>
@@ -2470,7 +2473,7 @@
       <c r="B29" s="41"/>
       <c r="C29" s="47"/>
       <c r="D29" s="28" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="E29" s="29"/>
       <c r="F29" s="29"/>
@@ -2503,17 +2506,14 @@
       <c r="AG29" s="29"/>
       <c r="AH29" s="29"/>
       <c r="AI29" s="29"/>
-      <c r="AJ29" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="AJ29" s="7"/>
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A30" s="44"/>
       <c r="B30" s="41"/>
       <c r="C30" s="47"/>
       <c r="D30" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E30" s="29"/>
       <c r="F30" s="29"/>
@@ -2556,7 +2556,7 @@
       <c r="B31" s="41"/>
       <c r="C31" s="47"/>
       <c r="D31" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E31" s="29"/>
       <c r="F31" s="29"/>
@@ -2599,7 +2599,7 @@
       <c r="B32" s="41"/>
       <c r="C32" s="47"/>
       <c r="D32" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E32" s="29"/>
       <c r="F32" s="29"/>
@@ -2642,7 +2642,7 @@
       <c r="B33" s="41"/>
       <c r="C33" s="47"/>
       <c r="D33" s="28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E33" s="29"/>
       <c r="F33" s="29"/>
@@ -2685,7 +2685,7 @@
       <c r="B34" s="41"/>
       <c r="C34" s="47"/>
       <c r="D34" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E34" s="29"/>
       <c r="F34" s="29"/>
@@ -2728,7 +2728,7 @@
       <c r="B35" s="41"/>
       <c r="C35" s="47"/>
       <c r="D35" s="28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E35" s="29"/>
       <c r="F35" s="29"/>
@@ -2771,7 +2771,7 @@
       <c r="B36" s="41"/>
       <c r="C36" s="47"/>
       <c r="D36" s="28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E36" s="29"/>
       <c r="F36" s="29"/>
@@ -2812,9 +2812,9 @@
     <row r="37" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A37" s="44"/>
       <c r="B37" s="41"/>
-      <c r="C37" s="48"/>
+      <c r="C37" s="47"/>
       <c r="D37" s="28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E37" s="29"/>
       <c r="F37" s="29"/>
@@ -2852,97 +2852,97 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A38" s="44"/>
       <c r="B38" s="41"/>
-      <c r="C38" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
-      <c r="L38" s="20"/>
-      <c r="M38" s="20"/>
-      <c r="N38" s="20"/>
-      <c r="O38" s="20"/>
-      <c r="P38" s="20"/>
-      <c r="Q38" s="20"/>
-      <c r="R38" s="20"/>
-      <c r="S38" s="20"/>
-      <c r="T38" s="20"/>
-      <c r="U38" s="20"/>
-      <c r="V38" s="20"/>
-      <c r="W38" s="20"/>
-      <c r="X38" s="20"/>
-      <c r="Y38" s="20"/>
-      <c r="Z38" s="20"/>
-      <c r="AA38" s="20"/>
-      <c r="AB38" s="20"/>
-      <c r="AC38" s="20"/>
-      <c r="AD38" s="20"/>
-      <c r="AE38" s="20"/>
-      <c r="AF38" s="20"/>
-      <c r="AG38" s="20"/>
-      <c r="AH38" s="20"/>
-      <c r="AI38" s="20"/>
-      <c r="AJ38" s="21"/>
-    </row>
-    <row r="39" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="48"/>
+      <c r="D38" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="29"/>
+      <c r="K38" s="29"/>
+      <c r="L38" s="29"/>
+      <c r="M38" s="29"/>
+      <c r="N38" s="29"/>
+      <c r="O38" s="29"/>
+      <c r="P38" s="29"/>
+      <c r="Q38" s="29"/>
+      <c r="R38" s="29"/>
+      <c r="S38" s="29"/>
+      <c r="T38" s="29"/>
+      <c r="U38" s="29"/>
+      <c r="V38" s="29"/>
+      <c r="W38" s="29"/>
+      <c r="X38" s="29"/>
+      <c r="Y38" s="29"/>
+      <c r="Z38" s="29"/>
+      <c r="AA38" s="29"/>
+      <c r="AB38" s="29"/>
+      <c r="AC38" s="29"/>
+      <c r="AD38" s="29"/>
+      <c r="AE38" s="29"/>
+      <c r="AF38" s="29"/>
+      <c r="AG38" s="29"/>
+      <c r="AH38" s="29"/>
+      <c r="AI38" s="29"/>
+      <c r="AJ38" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="44"/>
       <c r="B39" s="41"/>
-      <c r="C39" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="30"/>
-      <c r="J39" s="30"/>
-      <c r="K39" s="30"/>
-      <c r="L39" s="30"/>
-      <c r="M39" s="30"/>
-      <c r="N39" s="30"/>
-      <c r="O39" s="30"/>
-      <c r="P39" s="30"/>
-      <c r="Q39" s="30"/>
-      <c r="R39" s="30"/>
-      <c r="S39" s="30"/>
-      <c r="T39" s="30"/>
-      <c r="U39" s="30"/>
-      <c r="V39" s="30"/>
-      <c r="W39" s="30"/>
-      <c r="X39" s="30"/>
-      <c r="Y39" s="30"/>
-      <c r="Z39" s="30"/>
-      <c r="AA39" s="30"/>
-      <c r="AB39" s="30"/>
-      <c r="AC39" s="30"/>
-      <c r="AD39" s="30"/>
-      <c r="AE39" s="30"/>
-      <c r="AF39" s="30"/>
-      <c r="AG39" s="30"/>
-      <c r="AH39" s="30"/>
-      <c r="AI39" s="30"/>
-      <c r="AJ39" s="34">
-        <f>SUM(E39:AI39)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C39" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
+      <c r="L39" s="20"/>
+      <c r="M39" s="20"/>
+      <c r="N39" s="20"/>
+      <c r="O39" s="20"/>
+      <c r="P39" s="20"/>
+      <c r="Q39" s="20"/>
+      <c r="R39" s="20"/>
+      <c r="S39" s="20"/>
+      <c r="T39" s="20"/>
+      <c r="U39" s="20"/>
+      <c r="V39" s="20"/>
+      <c r="W39" s="20"/>
+      <c r="X39" s="20"/>
+      <c r="Y39" s="20"/>
+      <c r="Z39" s="20"/>
+      <c r="AA39" s="20"/>
+      <c r="AB39" s="20"/>
+      <c r="AC39" s="20"/>
+      <c r="AD39" s="20"/>
+      <c r="AE39" s="20"/>
+      <c r="AF39" s="20"/>
+      <c r="AG39" s="20"/>
+      <c r="AH39" s="20"/>
+      <c r="AI39" s="20"/>
+      <c r="AJ39" s="21"/>
+    </row>
+    <row r="40" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="44"/>
       <c r="B40" s="41"/>
-      <c r="C40" s="50"/>
+      <c r="C40" s="49" t="s">
+        <v>44</v>
+      </c>
       <c r="D40" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E40" s="30"/>
       <c r="F40" s="30"/>
@@ -2976,61 +2976,61 @@
       <c r="AH40" s="30"/>
       <c r="AI40" s="30"/>
       <c r="AJ40" s="34">
-        <f t="shared" ref="AJ40:AJ99" si="1">SUM(E40:AI40)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+        <f>SUM(E40:AI40)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="44"/>
       <c r="B41" s="41"/>
-      <c r="C41" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
-      <c r="I41" s="25"/>
-      <c r="J41" s="25"/>
-      <c r="K41" s="25"/>
-      <c r="L41" s="25"/>
-      <c r="M41" s="25"/>
-      <c r="N41" s="25"/>
-      <c r="O41" s="25"/>
-      <c r="P41" s="25"/>
-      <c r="Q41" s="25"/>
-      <c r="R41" s="25"/>
-      <c r="S41" s="25"/>
-      <c r="T41" s="25"/>
-      <c r="U41" s="25"/>
-      <c r="V41" s="25"/>
-      <c r="W41" s="25"/>
-      <c r="X41" s="25"/>
-      <c r="Y41" s="25"/>
-      <c r="Z41" s="25"/>
-      <c r="AA41" s="25"/>
-      <c r="AB41" s="25"/>
-      <c r="AC41" s="25"/>
-      <c r="AD41" s="25"/>
-      <c r="AE41" s="25"/>
-      <c r="AF41" s="25"/>
-      <c r="AG41" s="25"/>
-      <c r="AH41" s="25"/>
-      <c r="AI41" s="25"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E41" s="30"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="30"/>
+      <c r="H41" s="30"/>
+      <c r="I41" s="30"/>
+      <c r="J41" s="30"/>
+      <c r="K41" s="30"/>
+      <c r="L41" s="30"/>
+      <c r="M41" s="30"/>
+      <c r="N41" s="30"/>
+      <c r="O41" s="30"/>
+      <c r="P41" s="30"/>
+      <c r="Q41" s="30"/>
+      <c r="R41" s="30"/>
+      <c r="S41" s="30"/>
+      <c r="T41" s="30"/>
+      <c r="U41" s="30"/>
+      <c r="V41" s="30"/>
+      <c r="W41" s="30"/>
+      <c r="X41" s="30"/>
+      <c r="Y41" s="30"/>
+      <c r="Z41" s="30"/>
+      <c r="AA41" s="30"/>
+      <c r="AB41" s="30"/>
+      <c r="AC41" s="30"/>
+      <c r="AD41" s="30"/>
+      <c r="AE41" s="30"/>
+      <c r="AF41" s="30"/>
+      <c r="AG41" s="30"/>
+      <c r="AH41" s="30"/>
+      <c r="AI41" s="30"/>
       <c r="AJ41" s="34">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+        <f t="shared" ref="AJ41:AJ100" si="1">SUM(E41:AI41)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="44"/>
       <c r="B42" s="41"/>
-      <c r="C42" s="52"/>
+      <c r="C42" s="51" t="s">
+        <v>47</v>
+      </c>
       <c r="D42" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E42" s="25"/>
       <c r="F42" s="25"/>
@@ -3073,7 +3073,7 @@
       <c r="B43" s="41"/>
       <c r="C43" s="52"/>
       <c r="D43" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E43" s="25"/>
       <c r="F43" s="25"/>
@@ -3114,9 +3114,9 @@
     <row r="44" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="44"/>
       <c r="B44" s="41"/>
-      <c r="C44" s="53"/>
+      <c r="C44" s="52"/>
       <c r="D44" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E44" s="25"/>
       <c r="F44" s="25"/>
@@ -3157,43 +3157,41 @@
     <row r="45" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="44"/>
       <c r="B45" s="41"/>
-      <c r="C45" s="54" t="s">
-        <v>52</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31"/>
-      <c r="H45" s="31"/>
-      <c r="I45" s="31"/>
-      <c r="J45" s="31"/>
-      <c r="K45" s="31"/>
-      <c r="L45" s="31"/>
-      <c r="M45" s="31"/>
-      <c r="N45" s="31"/>
-      <c r="O45" s="31"/>
-      <c r="P45" s="31"/>
-      <c r="Q45" s="31"/>
-      <c r="R45" s="31"/>
-      <c r="S45" s="31"/>
-      <c r="T45" s="31"/>
-      <c r="U45" s="31"/>
-      <c r="V45" s="31"/>
-      <c r="W45" s="31"/>
-      <c r="X45" s="31"/>
-      <c r="Y45" s="31"/>
-      <c r="Z45" s="31"/>
-      <c r="AA45" s="31"/>
-      <c r="AB45" s="31"/>
-      <c r="AC45" s="31"/>
-      <c r="AD45" s="31"/>
-      <c r="AE45" s="31"/>
-      <c r="AF45" s="31"/>
-      <c r="AG45" s="31"/>
-      <c r="AH45" s="31"/>
-      <c r="AI45" s="31"/>
+      <c r="C45" s="53"/>
+      <c r="D45" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E45" s="25"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="25"/>
+      <c r="H45" s="25"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="25"/>
+      <c r="K45" s="25"/>
+      <c r="L45" s="25"/>
+      <c r="M45" s="25"/>
+      <c r="N45" s="25"/>
+      <c r="O45" s="25"/>
+      <c r="P45" s="25"/>
+      <c r="Q45" s="25"/>
+      <c r="R45" s="25"/>
+      <c r="S45" s="25"/>
+      <c r="T45" s="25"/>
+      <c r="U45" s="25"/>
+      <c r="V45" s="25"/>
+      <c r="W45" s="25"/>
+      <c r="X45" s="25"/>
+      <c r="Y45" s="25"/>
+      <c r="Z45" s="25"/>
+      <c r="AA45" s="25"/>
+      <c r="AB45" s="25"/>
+      <c r="AC45" s="25"/>
+      <c r="AD45" s="25"/>
+      <c r="AE45" s="25"/>
+      <c r="AF45" s="25"/>
+      <c r="AG45" s="25"/>
+      <c r="AH45" s="25"/>
+      <c r="AI45" s="25"/>
       <c r="AJ45" s="34">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3202,9 +3200,11 @@
     <row r="46" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="44"/>
       <c r="B46" s="41"/>
-      <c r="C46" s="55"/>
+      <c r="C46" s="54" t="s">
+        <v>52</v>
+      </c>
       <c r="D46" s="12" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="E46" s="31"/>
       <c r="F46" s="31"/>
@@ -3247,7 +3247,7 @@
       <c r="B47" s="41"/>
       <c r="C47" s="55"/>
       <c r="D47" s="12" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="E47" s="31"/>
       <c r="F47" s="31"/>
@@ -3290,7 +3290,7 @@
       <c r="B48" s="41"/>
       <c r="C48" s="55"/>
       <c r="D48" s="12" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="E48" s="31"/>
       <c r="F48" s="31"/>
@@ -3333,7 +3333,7 @@
       <c r="B49" s="41"/>
       <c r="C49" s="55"/>
       <c r="D49" s="12" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="E49" s="31"/>
       <c r="F49" s="31"/>
@@ -3374,9 +3374,9 @@
     <row r="50" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="44"/>
       <c r="B50" s="41"/>
-      <c r="C50" s="56"/>
+      <c r="C50" s="55"/>
       <c r="D50" s="12" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="E50" s="31"/>
       <c r="F50" s="31"/>
@@ -3414,91 +3414,89 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:36" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="44"/>
       <c r="B51" s="41"/>
-      <c r="C51" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D51" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
-      <c r="I51" s="8"/>
-      <c r="J51" s="8"/>
-      <c r="K51" s="8"/>
-      <c r="L51" s="8"/>
-      <c r="M51" s="8"/>
-      <c r="N51" s="8"/>
-      <c r="O51" s="8"/>
-      <c r="P51" s="8"/>
-      <c r="Q51" s="8"/>
-      <c r="R51" s="8"/>
-      <c r="S51" s="8"/>
-      <c r="T51" s="8"/>
-      <c r="U51" s="8"/>
-      <c r="V51" s="8"/>
-      <c r="W51" s="8"/>
-      <c r="X51" s="8"/>
-      <c r="Y51" s="8"/>
-      <c r="Z51" s="8"/>
-      <c r="AA51" s="8"/>
-      <c r="AB51" s="8"/>
-      <c r="AC51" s="8"/>
-      <c r="AD51" s="8"/>
-      <c r="AE51" s="8"/>
-      <c r="AF51" s="8"/>
-      <c r="AG51" s="8"/>
-      <c r="AH51" s="8"/>
-      <c r="AI51" s="8"/>
+      <c r="C51" s="56"/>
+      <c r="D51" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E51" s="31"/>
+      <c r="F51" s="31"/>
+      <c r="G51" s="31"/>
+      <c r="H51" s="31"/>
+      <c r="I51" s="31"/>
+      <c r="J51" s="31"/>
+      <c r="K51" s="31"/>
+      <c r="L51" s="31"/>
+      <c r="M51" s="31"/>
+      <c r="N51" s="31"/>
+      <c r="O51" s="31"/>
+      <c r="P51" s="31"/>
+      <c r="Q51" s="31"/>
+      <c r="R51" s="31"/>
+      <c r="S51" s="31"/>
+      <c r="T51" s="31"/>
+      <c r="U51" s="31"/>
+      <c r="V51" s="31"/>
+      <c r="W51" s="31"/>
+      <c r="X51" s="31"/>
+      <c r="Y51" s="31"/>
+      <c r="Z51" s="31"/>
+      <c r="AA51" s="31"/>
+      <c r="AB51" s="31"/>
+      <c r="AC51" s="31"/>
+      <c r="AD51" s="31"/>
+      <c r="AE51" s="31"/>
+      <c r="AF51" s="31"/>
+      <c r="AG51" s="31"/>
+      <c r="AH51" s="31"/>
+      <c r="AI51" s="31"/>
       <c r="AJ51" s="34">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:36" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A52" s="44"/>
       <c r="B52" s="41"/>
-      <c r="C52" s="57" t="s">
-        <v>58</v>
-      </c>
-      <c r="D52" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="E52" s="27"/>
-      <c r="F52" s="27"/>
-      <c r="G52" s="27"/>
-      <c r="H52" s="27"/>
-      <c r="I52" s="27"/>
-      <c r="J52" s="27"/>
-      <c r="K52" s="27"/>
-      <c r="L52" s="27"/>
-      <c r="M52" s="27"/>
-      <c r="N52" s="27"/>
-      <c r="O52" s="27"/>
-      <c r="P52" s="27"/>
-      <c r="Q52" s="27"/>
-      <c r="R52" s="27"/>
-      <c r="S52" s="27"/>
-      <c r="T52" s="27"/>
-      <c r="U52" s="27"/>
-      <c r="V52" s="27"/>
-      <c r="W52" s="27"/>
-      <c r="X52" s="27"/>
-      <c r="Y52" s="27"/>
-      <c r="Z52" s="27"/>
-      <c r="AA52" s="27"/>
-      <c r="AB52" s="27"/>
-      <c r="AC52" s="27"/>
-      <c r="AD52" s="27"/>
-      <c r="AE52" s="27"/>
-      <c r="AF52" s="27"/>
-      <c r="AG52" s="27"/>
-      <c r="AH52" s="27"/>
-      <c r="AI52" s="27"/>
+      <c r="C52" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D52" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="8"/>
+      <c r="L52" s="8"/>
+      <c r="M52" s="8"/>
+      <c r="N52" s="8"/>
+      <c r="O52" s="8"/>
+      <c r="P52" s="8"/>
+      <c r="Q52" s="8"/>
+      <c r="R52" s="8"/>
+      <c r="S52" s="8"/>
+      <c r="T52" s="8"/>
+      <c r="U52" s="8"/>
+      <c r="V52" s="8"/>
+      <c r="W52" s="8"/>
+      <c r="X52" s="8"/>
+      <c r="Y52" s="8"/>
+      <c r="Z52" s="8"/>
+      <c r="AA52" s="8"/>
+      <c r="AB52" s="8"/>
+      <c r="AC52" s="8"/>
+      <c r="AD52" s="8"/>
+      <c r="AE52" s="8"/>
+      <c r="AF52" s="8"/>
+      <c r="AG52" s="8"/>
+      <c r="AH52" s="8"/>
+      <c r="AI52" s="8"/>
       <c r="AJ52" s="34">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3507,9 +3505,11 @@
     <row r="53" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="44"/>
       <c r="B53" s="41"/>
-      <c r="C53" s="58"/>
+      <c r="C53" s="57" t="s">
+        <v>58</v>
+      </c>
       <c r="D53" s="14" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="E53" s="27"/>
       <c r="F53" s="27"/>
@@ -3542,14 +3542,17 @@
       <c r="AG53" s="27"/>
       <c r="AH53" s="27"/>
       <c r="AI53" s="27"/>
-      <c r="AJ53" s="34"/>
-    </row>
-    <row r="54" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AJ53" s="34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="44"/>
       <c r="B54" s="41"/>
       <c r="C54" s="58"/>
       <c r="D54" s="14" t="s">
-        <v>25</v>
+        <v>95</v>
       </c>
       <c r="E54" s="27"/>
       <c r="F54" s="27"/>
@@ -3582,17 +3585,14 @@
       <c r="AG54" s="27"/>
       <c r="AH54" s="27"/>
       <c r="AI54" s="27"/>
-      <c r="AJ54" s="34">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="AJ54" s="34"/>
     </row>
     <row r="55" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="44"/>
       <c r="B55" s="41"/>
       <c r="C55" s="58"/>
       <c r="D55" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E55" s="27"/>
       <c r="F55" s="27"/>
@@ -3635,7 +3635,7 @@
       <c r="B56" s="41"/>
       <c r="C56" s="58"/>
       <c r="D56" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E56" s="27"/>
       <c r="F56" s="27"/>
@@ -3678,7 +3678,7 @@
       <c r="B57" s="41"/>
       <c r="C57" s="58"/>
       <c r="D57" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E57" s="27"/>
       <c r="F57" s="27"/>
@@ -3721,7 +3721,7 @@
       <c r="B58" s="41"/>
       <c r="C58" s="58"/>
       <c r="D58" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E58" s="27"/>
       <c r="F58" s="27"/>
@@ -3764,7 +3764,7 @@
       <c r="B59" s="41"/>
       <c r="C59" s="58"/>
       <c r="D59" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E59" s="27"/>
       <c r="F59" s="27"/>
@@ -3807,7 +3807,7 @@
       <c r="B60" s="41"/>
       <c r="C60" s="58"/>
       <c r="D60" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E60" s="27"/>
       <c r="F60" s="27"/>
@@ -3850,7 +3850,7 @@
       <c r="B61" s="41"/>
       <c r="C61" s="58"/>
       <c r="D61" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E61" s="27"/>
       <c r="F61" s="27"/>
@@ -3893,7 +3893,7 @@
       <c r="B62" s="41"/>
       <c r="C62" s="58"/>
       <c r="D62" s="14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E62" s="27"/>
       <c r="F62" s="27"/>
@@ -3936,7 +3936,7 @@
       <c r="B63" s="41"/>
       <c r="C63" s="58"/>
       <c r="D63" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E63" s="27"/>
       <c r="F63" s="27"/>
@@ -3979,7 +3979,7 @@
       <c r="B64" s="41"/>
       <c r="C64" s="58"/>
       <c r="D64" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E64" s="27"/>
       <c r="F64" s="27"/>
@@ -4022,7 +4022,7 @@
       <c r="B65" s="41"/>
       <c r="C65" s="58"/>
       <c r="D65" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E65" s="27"/>
       <c r="F65" s="27"/>
@@ -4065,7 +4065,7 @@
       <c r="B66" s="41"/>
       <c r="C66" s="58"/>
       <c r="D66" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E66" s="27"/>
       <c r="F66" s="27"/>
@@ -4106,9 +4106,9 @@
     <row r="67" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="44"/>
       <c r="B67" s="41"/>
-      <c r="C67" s="59"/>
+      <c r="C67" s="58"/>
       <c r="D67" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E67" s="27"/>
       <c r="F67" s="27"/>
@@ -4149,43 +4149,41 @@
     <row r="68" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="44"/>
       <c r="B68" s="41"/>
-      <c r="C68" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="D68" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E68" s="32"/>
-      <c r="F68" s="32"/>
-      <c r="G68" s="32"/>
-      <c r="H68" s="32"/>
-      <c r="I68" s="32"/>
-      <c r="J68" s="32"/>
-      <c r="K68" s="32"/>
-      <c r="L68" s="32"/>
-      <c r="M68" s="32"/>
-      <c r="N68" s="32"/>
-      <c r="O68" s="32"/>
-      <c r="P68" s="32"/>
-      <c r="Q68" s="32"/>
-      <c r="R68" s="32"/>
-      <c r="S68" s="32"/>
-      <c r="T68" s="32"/>
-      <c r="U68" s="32"/>
-      <c r="V68" s="32"/>
-      <c r="W68" s="32"/>
-      <c r="X68" s="32"/>
-      <c r="Y68" s="32"/>
-      <c r="Z68" s="32"/>
-      <c r="AA68" s="32"/>
-      <c r="AB68" s="32"/>
-      <c r="AC68" s="32"/>
-      <c r="AD68" s="32"/>
-      <c r="AE68" s="32"/>
-      <c r="AF68" s="32"/>
-      <c r="AG68" s="32"/>
-      <c r="AH68" s="32"/>
-      <c r="AI68" s="32"/>
+      <c r="C68" s="59"/>
+      <c r="D68" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E68" s="27"/>
+      <c r="F68" s="27"/>
+      <c r="G68" s="27"/>
+      <c r="H68" s="27"/>
+      <c r="I68" s="27"/>
+      <c r="J68" s="27"/>
+      <c r="K68" s="27"/>
+      <c r="L68" s="27"/>
+      <c r="M68" s="27"/>
+      <c r="N68" s="27"/>
+      <c r="O68" s="27"/>
+      <c r="P68" s="27"/>
+      <c r="Q68" s="27"/>
+      <c r="R68" s="27"/>
+      <c r="S68" s="27"/>
+      <c r="T68" s="27"/>
+      <c r="U68" s="27"/>
+      <c r="V68" s="27"/>
+      <c r="W68" s="27"/>
+      <c r="X68" s="27"/>
+      <c r="Y68" s="27"/>
+      <c r="Z68" s="27"/>
+      <c r="AA68" s="27"/>
+      <c r="AB68" s="27"/>
+      <c r="AC68" s="27"/>
+      <c r="AD68" s="27"/>
+      <c r="AE68" s="27"/>
+      <c r="AF68" s="27"/>
+      <c r="AG68" s="27"/>
+      <c r="AH68" s="27"/>
+      <c r="AI68" s="27"/>
       <c r="AJ68" s="34">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4194,9 +4192,11 @@
     <row r="69" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="44"/>
       <c r="B69" s="41"/>
-      <c r="C69" s="38"/>
-      <c r="D69" s="16" t="s">
-        <v>62</v>
+      <c r="C69" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="D69" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="E69" s="32"/>
       <c r="F69" s="32"/>
@@ -4239,7 +4239,7 @@
       <c r="B70" s="41"/>
       <c r="C70" s="38"/>
       <c r="D70" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E70" s="32"/>
       <c r="F70" s="32"/>
@@ -4282,7 +4282,7 @@
       <c r="B71" s="41"/>
       <c r="C71" s="38"/>
       <c r="D71" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E71" s="32"/>
       <c r="F71" s="32"/>
@@ -4325,7 +4325,7 @@
       <c r="B72" s="41"/>
       <c r="C72" s="38"/>
       <c r="D72" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E72" s="32"/>
       <c r="F72" s="32"/>
@@ -4368,7 +4368,7 @@
       <c r="B73" s="41"/>
       <c r="C73" s="38"/>
       <c r="D73" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E73" s="32"/>
       <c r="F73" s="32"/>
@@ -4411,7 +4411,7 @@
       <c r="B74" s="41"/>
       <c r="C74" s="38"/>
       <c r="D74" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E74" s="32"/>
       <c r="F74" s="32"/>
@@ -4454,7 +4454,7 @@
       <c r="B75" s="41"/>
       <c r="C75" s="38"/>
       <c r="D75" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E75" s="32"/>
       <c r="F75" s="32"/>
@@ -4497,7 +4497,7 @@
       <c r="B76" s="41"/>
       <c r="C76" s="38"/>
       <c r="D76" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E76" s="32"/>
       <c r="F76" s="32"/>
@@ -4540,7 +4540,7 @@
       <c r="B77" s="41"/>
       <c r="C77" s="38"/>
       <c r="D77" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E77" s="32"/>
       <c r="F77" s="32"/>
@@ -4583,7 +4583,7 @@
       <c r="B78" s="41"/>
       <c r="C78" s="38"/>
       <c r="D78" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E78" s="32"/>
       <c r="F78" s="32"/>
@@ -4626,7 +4626,7 @@
       <c r="B79" s="41"/>
       <c r="C79" s="38"/>
       <c r="D79" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E79" s="32"/>
       <c r="F79" s="32"/>
@@ -4669,7 +4669,7 @@
       <c r="B80" s="41"/>
       <c r="C80" s="38"/>
       <c r="D80" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E80" s="32"/>
       <c r="F80" s="32"/>
@@ -4712,7 +4712,7 @@
       <c r="B81" s="41"/>
       <c r="C81" s="38"/>
       <c r="D81" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E81" s="32"/>
       <c r="F81" s="32"/>
@@ -4755,7 +4755,7 @@
       <c r="B82" s="41"/>
       <c r="C82" s="38"/>
       <c r="D82" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E82" s="32"/>
       <c r="F82" s="32"/>
@@ -4798,7 +4798,7 @@
       <c r="B83" s="41"/>
       <c r="C83" s="38"/>
       <c r="D83" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E83" s="32"/>
       <c r="F83" s="32"/>
@@ -4841,7 +4841,7 @@
       <c r="B84" s="41"/>
       <c r="C84" s="38"/>
       <c r="D84" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E84" s="32"/>
       <c r="F84" s="32"/>
@@ -4884,7 +4884,7 @@
       <c r="B85" s="41"/>
       <c r="C85" s="38"/>
       <c r="D85" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E85" s="32"/>
       <c r="F85" s="32"/>
@@ -4927,7 +4927,7 @@
       <c r="B86" s="41"/>
       <c r="C86" s="38"/>
       <c r="D86" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E86" s="32"/>
       <c r="F86" s="32"/>
@@ -4970,7 +4970,7 @@
       <c r="B87" s="41"/>
       <c r="C87" s="38"/>
       <c r="D87" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E87" s="32"/>
       <c r="F87" s="32"/>
@@ -5013,7 +5013,7 @@
       <c r="B88" s="41"/>
       <c r="C88" s="38"/>
       <c r="D88" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E88" s="32"/>
       <c r="F88" s="32"/>
@@ -5056,7 +5056,7 @@
       <c r="B89" s="41"/>
       <c r="C89" s="38"/>
       <c r="D89" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E89" s="32"/>
       <c r="F89" s="32"/>
@@ -5099,7 +5099,7 @@
       <c r="B90" s="41"/>
       <c r="C90" s="38"/>
       <c r="D90" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E90" s="32"/>
       <c r="F90" s="32"/>
@@ -5142,7 +5142,7 @@
       <c r="B91" s="41"/>
       <c r="C91" s="38"/>
       <c r="D91" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E91" s="32"/>
       <c r="F91" s="32"/>
@@ -5185,7 +5185,7 @@
       <c r="B92" s="41"/>
       <c r="C92" s="38"/>
       <c r="D92" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E92" s="32"/>
       <c r="F92" s="32"/>
@@ -5228,7 +5228,7 @@
       <c r="B93" s="41"/>
       <c r="C93" s="38"/>
       <c r="D93" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E93" s="32"/>
       <c r="F93" s="32"/>
@@ -5271,7 +5271,7 @@
       <c r="B94" s="41"/>
       <c r="C94" s="38"/>
       <c r="D94" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E94" s="32"/>
       <c r="F94" s="32"/>
@@ -5314,7 +5314,7 @@
       <c r="B95" s="41"/>
       <c r="C95" s="38"/>
       <c r="D95" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E95" s="32"/>
       <c r="F95" s="32"/>
@@ -5357,7 +5357,7 @@
       <c r="B96" s="41"/>
       <c r="C96" s="38"/>
       <c r="D96" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E96" s="32"/>
       <c r="F96" s="32"/>
@@ -5400,7 +5400,7 @@
       <c r="B97" s="41"/>
       <c r="C97" s="38"/>
       <c r="D97" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E97" s="32"/>
       <c r="F97" s="32"/>
@@ -5442,8 +5442,8 @@
       <c r="A98" s="44"/>
       <c r="B98" s="41"/>
       <c r="C98" s="38"/>
-      <c r="D98" s="17" t="s">
-        <v>91</v>
+      <c r="D98" s="16" t="s">
+        <v>90</v>
       </c>
       <c r="E98" s="32"/>
       <c r="F98" s="32"/>
@@ -5481,68 +5481,111 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:36" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="45"/>
-      <c r="B99" s="42"/>
-      <c r="C99" s="39"/>
-      <c r="D99" s="18" t="s">
+    <row r="99" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A99" s="44"/>
+      <c r="B99" s="41"/>
+      <c r="C99" s="38"/>
+      <c r="D99" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E99" s="32"/>
+      <c r="F99" s="32"/>
+      <c r="G99" s="32"/>
+      <c r="H99" s="32"/>
+      <c r="I99" s="32"/>
+      <c r="J99" s="32"/>
+      <c r="K99" s="32"/>
+      <c r="L99" s="32"/>
+      <c r="M99" s="32"/>
+      <c r="N99" s="32"/>
+      <c r="O99" s="32"/>
+      <c r="P99" s="32"/>
+      <c r="Q99" s="32"/>
+      <c r="R99" s="32"/>
+      <c r="S99" s="32"/>
+      <c r="T99" s="32"/>
+      <c r="U99" s="32"/>
+      <c r="V99" s="32"/>
+      <c r="W99" s="32"/>
+      <c r="X99" s="32"/>
+      <c r="Y99" s="32"/>
+      <c r="Z99" s="32"/>
+      <c r="AA99" s="32"/>
+      <c r="AB99" s="32"/>
+      <c r="AC99" s="32"/>
+      <c r="AD99" s="32"/>
+      <c r="AE99" s="32"/>
+      <c r="AF99" s="32"/>
+      <c r="AG99" s="32"/>
+      <c r="AH99" s="32"/>
+      <c r="AI99" s="32"/>
+      <c r="AJ99" s="34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:36" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="45"/>
+      <c r="B100" s="42"/>
+      <c r="C100" s="39"/>
+      <c r="D100" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="E99" s="33"/>
-      <c r="F99" s="33"/>
-      <c r="G99" s="33"/>
-      <c r="H99" s="33"/>
-      <c r="I99" s="33"/>
-      <c r="J99" s="33"/>
-      <c r="K99" s="33"/>
-      <c r="L99" s="33"/>
-      <c r="M99" s="33"/>
-      <c r="N99" s="33"/>
-      <c r="O99" s="33"/>
-      <c r="P99" s="33"/>
-      <c r="Q99" s="33"/>
-      <c r="R99" s="33"/>
-      <c r="S99" s="33"/>
-      <c r="T99" s="33"/>
-      <c r="U99" s="33"/>
-      <c r="V99" s="33"/>
-      <c r="W99" s="33"/>
-      <c r="X99" s="33"/>
-      <c r="Y99" s="33"/>
-      <c r="Z99" s="33"/>
-      <c r="AA99" s="33"/>
-      <c r="AB99" s="33"/>
-      <c r="AC99" s="33"/>
-      <c r="AD99" s="33"/>
-      <c r="AE99" s="33"/>
-      <c r="AF99" s="33"/>
-      <c r="AG99" s="33"/>
-      <c r="AH99" s="33"/>
-      <c r="AI99" s="33"/>
-      <c r="AJ99" s="34">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="AI100" s="36" t="s">
+      <c r="E100" s="33"/>
+      <c r="F100" s="33"/>
+      <c r="G100" s="33"/>
+      <c r="H100" s="33"/>
+      <c r="I100" s="33"/>
+      <c r="J100" s="33"/>
+      <c r="K100" s="33"/>
+      <c r="L100" s="33"/>
+      <c r="M100" s="33"/>
+      <c r="N100" s="33"/>
+      <c r="O100" s="33"/>
+      <c r="P100" s="33"/>
+      <c r="Q100" s="33"/>
+      <c r="R100" s="33"/>
+      <c r="S100" s="33"/>
+      <c r="T100" s="33"/>
+      <c r="U100" s="33"/>
+      <c r="V100" s="33"/>
+      <c r="W100" s="33"/>
+      <c r="X100" s="33"/>
+      <c r="Y100" s="33"/>
+      <c r="Z100" s="33"/>
+      <c r="AA100" s="33"/>
+      <c r="AB100" s="33"/>
+      <c r="AC100" s="33"/>
+      <c r="AD100" s="33"/>
+      <c r="AE100" s="33"/>
+      <c r="AF100" s="33"/>
+      <c r="AG100" s="33"/>
+      <c r="AH100" s="33"/>
+      <c r="AI100" s="33"/>
+      <c r="AJ100" s="34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="AI101" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="AJ100" s="35">
-        <f>SUM(AJ2:AJ99)</f>
+      <c r="AJ101" s="35">
+        <f>SUM(AJ2:AJ100)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C68:C99"/>
-    <mergeCell ref="B1:B99"/>
-    <mergeCell ref="A1:A99"/>
-    <mergeCell ref="C18:C37"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C41:C44"/>
-    <mergeCell ref="C45:C50"/>
-    <mergeCell ref="C52:C67"/>
+    <mergeCell ref="C69:C100"/>
+    <mergeCell ref="B1:B100"/>
+    <mergeCell ref="A1:A100"/>
+    <mergeCell ref="C18:C38"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="C46:C51"/>
+    <mergeCell ref="C53:C68"/>
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="C6:C14"/>
     <mergeCell ref="C16:C17"/>

</xml_diff>

<commit_message>
[UPDATE] - Monthly Report MK Spesial & Snack, previous data
</commit_message>
<xml_diff>
--- a/resources/template/BINTANG.xlsx
+++ b/resources/template/BINTANG.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hallo_ppa\resources\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDE2802-3816-4286-AA5E-0277AF9C18E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF60E27-D270-4FD5-9D4D-1F156D54301F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{96DAB095-C63E-43E2-9BFC-56E2EB8E01C9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Reguler" sheetId="1" r:id="rId1"/>
+    <sheet name="Snack" sheetId="5" r:id="rId2"/>
+    <sheet name="Spesial" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -710,7 +712,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -820,99 +822,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -934,6 +843,105 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1256,22 +1264,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{727E0051-6F26-4AB8-8E1A-F7C7AFECA816}">
   <dimension ref="A1:AK173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="D125" sqref="D125"/>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.88671875" style="76"/>
-    <col min="3" max="3" width="32.33203125" style="76" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="45"/>
+    <col min="3" max="3" width="32.33203125" style="45" customWidth="1"/>
     <col min="4" max="4" width="44.109375" customWidth="1"/>
     <col min="5" max="5" width="9" style="35" customWidth="1"/>
     <col min="6" max="35" width="8.88671875" style="35"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="45"/>
-      <c r="B1" s="42"/>
+      <c r="A1" s="57"/>
+      <c r="B1" s="54"/>
       <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
@@ -1377,9 +1385,9 @@
       <c r="AK1" s="3"/>
     </row>
     <row r="2" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="46"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="51" t="s">
+      <c r="A2" s="58"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="63" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="21" t="s">
@@ -1423,9 +1431,9 @@
       <c r="AK2" s="2"/>
     </row>
     <row r="3" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="46"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="62"/>
+      <c r="A3" s="58"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="74"/>
       <c r="D3" s="21" t="s">
         <v>5</v>
       </c>
@@ -1467,9 +1475,9 @@
       <c r="AK3" s="2"/>
     </row>
     <row r="4" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="46"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="62"/>
+      <c r="A4" s="58"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="74"/>
       <c r="D4" s="21" t="s">
         <v>6</v>
       </c>
@@ -1511,9 +1519,9 @@
       <c r="AK4" s="2"/>
     </row>
     <row r="5" spans="1:37" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="46"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="52"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="64"/>
       <c r="D5" s="21" t="s">
         <v>7</v>
       </c>
@@ -1555,9 +1563,9 @@
       <c r="AK5" s="2"/>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A6" s="46"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="63" t="s">
+      <c r="A6" s="58"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="75" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="22" t="s">
@@ -1600,9 +1608,9 @@
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A7" s="46"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="64"/>
+      <c r="A7" s="58"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="76"/>
       <c r="D7" s="22" t="s">
         <v>10</v>
       </c>
@@ -1643,9 +1651,9 @@
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A8" s="46"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="64"/>
+      <c r="A8" s="58"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="76"/>
       <c r="D8" s="22" t="s">
         <v>11</v>
       </c>
@@ -1686,9 +1694,9 @@
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A9" s="46"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="64"/>
+      <c r="A9" s="58"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="76"/>
       <c r="D9" s="22" t="s">
         <v>12</v>
       </c>
@@ -1729,9 +1737,9 @@
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A10" s="46"/>
-      <c r="B10" s="43"/>
-      <c r="C10" s="64"/>
+      <c r="A10" s="58"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="76"/>
       <c r="D10" s="22" t="s">
         <v>13</v>
       </c>
@@ -1772,9 +1780,9 @@
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A11" s="46"/>
-      <c r="B11" s="43"/>
-      <c r="C11" s="64"/>
+      <c r="A11" s="58"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="76"/>
       <c r="D11" s="22" t="s">
         <v>14</v>
       </c>
@@ -1815,9 +1823,9 @@
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A12" s="46"/>
-      <c r="B12" s="43"/>
-      <c r="C12" s="64"/>
+      <c r="A12" s="58"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="76"/>
       <c r="D12" s="22" t="s">
         <v>15</v>
       </c>
@@ -1858,9 +1866,9 @@
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A13" s="46"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="64"/>
+      <c r="A13" s="58"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="76"/>
       <c r="D13" s="22" t="s">
         <v>16</v>
       </c>
@@ -1901,9 +1909,9 @@
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A14" s="46"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="65"/>
+      <c r="A14" s="58"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="77"/>
       <c r="D14" s="22" t="s">
         <v>89</v>
       </c>
@@ -1944,8 +1952,8 @@
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A15" s="46"/>
-      <c r="B15" s="43"/>
+      <c r="A15" s="58"/>
+      <c r="B15" s="55"/>
       <c r="C15" s="8" t="s">
         <v>18</v>
       </c>
@@ -1989,9 +1997,9 @@
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A16" s="46"/>
-      <c r="B16" s="43"/>
-      <c r="C16" s="66" t="s">
+      <c r="A16" s="58"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="78" t="s">
         <v>20</v>
       </c>
       <c r="D16" s="24" t="s">
@@ -2034,9 +2042,9 @@
       </c>
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A17" s="46"/>
-      <c r="B17" s="43"/>
-      <c r="C17" s="67"/>
+      <c r="A17" s="58"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="79"/>
       <c r="D17" s="24" t="s">
         <v>22</v>
       </c>
@@ -2077,9 +2085,9 @@
       </c>
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A18" s="46"/>
-      <c r="B18" s="43"/>
-      <c r="C18" s="48" t="s">
+      <c r="A18" s="58"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="60" t="s">
         <v>23</v>
       </c>
       <c r="D18" s="25" t="s">
@@ -2122,9 +2130,9 @@
       </c>
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A19" s="46"/>
-      <c r="B19" s="43"/>
-      <c r="C19" s="49"/>
+      <c r="A19" s="58"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="61"/>
       <c r="D19" s="25" t="s">
         <v>90</v>
       </c>
@@ -2162,9 +2170,9 @@
       <c r="AJ19" s="7"/>
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A20" s="46"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="49"/>
+      <c r="A20" s="58"/>
+      <c r="B20" s="55"/>
+      <c r="C20" s="61"/>
       <c r="D20" s="25" t="s">
         <v>25</v>
       </c>
@@ -2205,9 +2213,9 @@
       </c>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A21" s="46"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="49"/>
+      <c r="A21" s="58"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="61"/>
       <c r="D21" s="25" t="s">
         <v>26</v>
       </c>
@@ -2248,9 +2256,9 @@
       </c>
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A22" s="46"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="49"/>
+      <c r="A22" s="58"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="61"/>
       <c r="D22" s="25" t="s">
         <v>27</v>
       </c>
@@ -2291,9 +2299,9 @@
       </c>
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A23" s="46"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="49"/>
+      <c r="A23" s="58"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="61"/>
       <c r="D23" s="25" t="s">
         <v>28</v>
       </c>
@@ -2334,9 +2342,9 @@
       </c>
     </row>
     <row r="24" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A24" s="46"/>
-      <c r="B24" s="43"/>
-      <c r="C24" s="49"/>
+      <c r="A24" s="58"/>
+      <c r="B24" s="55"/>
+      <c r="C24" s="61"/>
       <c r="D24" s="25" t="s">
         <v>29</v>
       </c>
@@ -2377,9 +2385,9 @@
       </c>
     </row>
     <row r="25" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A25" s="46"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="49"/>
+      <c r="A25" s="58"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="61"/>
       <c r="D25" s="25" t="s">
         <v>30</v>
       </c>
@@ -2420,9 +2428,9 @@
       </c>
     </row>
     <row r="26" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A26" s="46"/>
-      <c r="B26" s="43"/>
-      <c r="C26" s="49"/>
+      <c r="A26" s="58"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="61"/>
       <c r="D26" s="25" t="s">
         <v>31</v>
       </c>
@@ -2463,9 +2471,9 @@
       </c>
     </row>
     <row r="27" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A27" s="46"/>
-      <c r="B27" s="43"/>
-      <c r="C27" s="49"/>
+      <c r="A27" s="58"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="61"/>
       <c r="D27" s="25" t="s">
         <v>32</v>
       </c>
@@ -2506,9 +2514,9 @@
       </c>
     </row>
     <row r="28" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A28" s="46"/>
-      <c r="B28" s="43"/>
-      <c r="C28" s="49"/>
+      <c r="A28" s="58"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="61"/>
       <c r="D28" s="25" t="s">
         <v>33</v>
       </c>
@@ -2549,9 +2557,9 @@
       </c>
     </row>
     <row r="29" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A29" s="46"/>
-      <c r="B29" s="43"/>
-      <c r="C29" s="49"/>
+      <c r="A29" s="58"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="61"/>
       <c r="D29" s="25" t="s">
         <v>92</v>
       </c>
@@ -2589,9 +2597,9 @@
       <c r="AJ29" s="7"/>
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A30" s="46"/>
-      <c r="B30" s="43"/>
-      <c r="C30" s="49"/>
+      <c r="A30" s="58"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="61"/>
       <c r="D30" s="25" t="s">
         <v>34</v>
       </c>
@@ -2632,9 +2640,9 @@
       </c>
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A31" s="46"/>
-      <c r="B31" s="43"/>
-      <c r="C31" s="49"/>
+      <c r="A31" s="58"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="61"/>
       <c r="D31" s="25" t="s">
         <v>35</v>
       </c>
@@ -2675,9 +2683,9 @@
       </c>
     </row>
     <row r="32" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A32" s="46"/>
-      <c r="B32" s="43"/>
-      <c r="C32" s="49"/>
+      <c r="A32" s="58"/>
+      <c r="B32" s="55"/>
+      <c r="C32" s="61"/>
       <c r="D32" s="25" t="s">
         <v>36</v>
       </c>
@@ -2718,9 +2726,9 @@
       </c>
     </row>
     <row r="33" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A33" s="46"/>
-      <c r="B33" s="43"/>
-      <c r="C33" s="49"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="55"/>
+      <c r="C33" s="61"/>
       <c r="D33" s="25" t="s">
         <v>37</v>
       </c>
@@ -2761,9 +2769,9 @@
       </c>
     </row>
     <row r="34" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A34" s="46"/>
-      <c r="B34" s="43"/>
-      <c r="C34" s="49"/>
+      <c r="A34" s="58"/>
+      <c r="B34" s="55"/>
+      <c r="C34" s="61"/>
       <c r="D34" s="25" t="s">
         <v>38</v>
       </c>
@@ -2804,9 +2812,9 @@
       </c>
     </row>
     <row r="35" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A35" s="46"/>
-      <c r="B35" s="43"/>
-      <c r="C35" s="49"/>
+      <c r="A35" s="58"/>
+      <c r="B35" s="55"/>
+      <c r="C35" s="61"/>
       <c r="D35" s="25" t="s">
         <v>39</v>
       </c>
@@ -2847,9 +2855,9 @@
       </c>
     </row>
     <row r="36" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A36" s="46"/>
-      <c r="B36" s="43"/>
-      <c r="C36" s="49"/>
+      <c r="A36" s="58"/>
+      <c r="B36" s="55"/>
+      <c r="C36" s="61"/>
       <c r="D36" s="25" t="s">
         <v>40</v>
       </c>
@@ -2890,9 +2898,9 @@
       </c>
     </row>
     <row r="37" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A37" s="46"/>
-      <c r="B37" s="43"/>
-      <c r="C37" s="49"/>
+      <c r="A37" s="58"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="61"/>
       <c r="D37" s="25" t="s">
         <v>41</v>
       </c>
@@ -2933,9 +2941,9 @@
       </c>
     </row>
     <row r="38" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A38" s="46"/>
-      <c r="B38" s="43"/>
-      <c r="C38" s="50"/>
+      <c r="A38" s="58"/>
+      <c r="B38" s="55"/>
+      <c r="C38" s="62"/>
       <c r="D38" s="25" t="s">
         <v>42</v>
       </c>
@@ -2976,8 +2984,8 @@
       </c>
     </row>
     <row r="39" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="46"/>
-      <c r="B39" s="43"/>
+      <c r="A39" s="58"/>
+      <c r="B39" s="55"/>
       <c r="C39" s="18" t="s">
         <v>43</v>
       </c>
@@ -3016,9 +3024,9 @@
       <c r="AJ39" s="20"/>
     </row>
     <row r="40" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="46"/>
-      <c r="B40" s="43"/>
-      <c r="C40" s="51" t="s">
+      <c r="A40" s="58"/>
+      <c r="B40" s="55"/>
+      <c r="C40" s="63" t="s">
         <v>44</v>
       </c>
       <c r="D40" s="9" t="s">
@@ -3061,9 +3069,9 @@
       </c>
     </row>
     <row r="41" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="46"/>
-      <c r="B41" s="43"/>
-      <c r="C41" s="52"/>
+      <c r="A41" s="58"/>
+      <c r="B41" s="55"/>
+      <c r="C41" s="64"/>
       <c r="D41" s="9" t="s">
         <v>46</v>
       </c>
@@ -3104,9 +3112,9 @@
       </c>
     </row>
     <row r="42" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="46"/>
-      <c r="B42" s="43"/>
-      <c r="C42" s="53" t="s">
+      <c r="A42" s="58"/>
+      <c r="B42" s="55"/>
+      <c r="C42" s="65" t="s">
         <v>47</v>
       </c>
       <c r="D42" s="10" t="s">
@@ -3149,9 +3157,9 @@
       </c>
     </row>
     <row r="43" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="46"/>
-      <c r="B43" s="43"/>
-      <c r="C43" s="54"/>
+      <c r="A43" s="58"/>
+      <c r="B43" s="55"/>
+      <c r="C43" s="66"/>
       <c r="D43" s="10" t="s">
         <v>49</v>
       </c>
@@ -3192,9 +3200,9 @@
       </c>
     </row>
     <row r="44" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="46"/>
-      <c r="B44" s="43"/>
-      <c r="C44" s="54"/>
+      <c r="A44" s="58"/>
+      <c r="B44" s="55"/>
+      <c r="C44" s="66"/>
       <c r="D44" s="10" t="s">
         <v>50</v>
       </c>
@@ -3235,9 +3243,9 @@
       </c>
     </row>
     <row r="45" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="46"/>
-      <c r="B45" s="43"/>
-      <c r="C45" s="55"/>
+      <c r="A45" s="58"/>
+      <c r="B45" s="55"/>
+      <c r="C45" s="67"/>
       <c r="D45" s="10" t="s">
         <v>51</v>
       </c>
@@ -3278,9 +3286,9 @@
       </c>
     </row>
     <row r="46" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="46"/>
-      <c r="B46" s="43"/>
-      <c r="C46" s="56" t="s">
+      <c r="A46" s="58"/>
+      <c r="B46" s="55"/>
+      <c r="C46" s="68" t="s">
         <v>52</v>
       </c>
       <c r="D46" s="11" t="s">
@@ -3323,9 +3331,9 @@
       </c>
     </row>
     <row r="47" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="46"/>
-      <c r="B47" s="43"/>
-      <c r="C47" s="57"/>
+      <c r="A47" s="58"/>
+      <c r="B47" s="55"/>
+      <c r="C47" s="69"/>
       <c r="D47" s="11" t="s">
         <v>16</v>
       </c>
@@ -3366,9 +3374,9 @@
       </c>
     </row>
     <row r="48" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="46"/>
-      <c r="B48" s="43"/>
-      <c r="C48" s="57"/>
+      <c r="A48" s="58"/>
+      <c r="B48" s="55"/>
+      <c r="C48" s="69"/>
       <c r="D48" s="11" t="s">
         <v>54</v>
       </c>
@@ -3409,9 +3417,9 @@
       </c>
     </row>
     <row r="49" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="46"/>
-      <c r="B49" s="43"/>
-      <c r="C49" s="57"/>
+      <c r="A49" s="58"/>
+      <c r="B49" s="55"/>
+      <c r="C49" s="69"/>
       <c r="D49" s="11" t="s">
         <v>21</v>
       </c>
@@ -3452,9 +3460,9 @@
       </c>
     </row>
     <row r="50" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="46"/>
-      <c r="B50" s="43"/>
-      <c r="C50" s="57"/>
+      <c r="A50" s="58"/>
+      <c r="B50" s="55"/>
+      <c r="C50" s="69"/>
       <c r="D50" s="11" t="s">
         <v>55</v>
       </c>
@@ -3495,9 +3503,9 @@
       </c>
     </row>
     <row r="51" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="46"/>
-      <c r="B51" s="43"/>
-      <c r="C51" s="58"/>
+      <c r="A51" s="58"/>
+      <c r="B51" s="55"/>
+      <c r="C51" s="70"/>
       <c r="D51" s="11" t="s">
         <v>17</v>
       </c>
@@ -3538,8 +3546,8 @@
       </c>
     </row>
     <row r="52" spans="1:36" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A52" s="46"/>
-      <c r="B52" s="43"/>
+      <c r="A52" s="58"/>
+      <c r="B52" s="55"/>
       <c r="C52" s="12" t="s">
         <v>56</v>
       </c>
@@ -3583,9 +3591,9 @@
       </c>
     </row>
     <row r="53" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="46"/>
-      <c r="B53" s="43"/>
-      <c r="C53" s="59" t="s">
+      <c r="A53" s="58"/>
+      <c r="B53" s="55"/>
+      <c r="C53" s="71" t="s">
         <v>58</v>
       </c>
       <c r="D53" s="13" t="s">
@@ -3628,9 +3636,9 @@
       </c>
     </row>
     <row r="54" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="46"/>
-      <c r="B54" s="43"/>
-      <c r="C54" s="60"/>
+      <c r="A54" s="58"/>
+      <c r="B54" s="55"/>
+      <c r="C54" s="72"/>
       <c r="D54" s="13" t="s">
         <v>91</v>
       </c>
@@ -3668,9 +3676,9 @@
       <c r="AJ54" s="26"/>
     </row>
     <row r="55" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="46"/>
-      <c r="B55" s="43"/>
-      <c r="C55" s="60"/>
+      <c r="A55" s="58"/>
+      <c r="B55" s="55"/>
+      <c r="C55" s="72"/>
       <c r="D55" s="13" t="s">
         <v>25</v>
       </c>
@@ -3711,9 +3719,9 @@
       </c>
     </row>
     <row r="56" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="46"/>
-      <c r="B56" s="43"/>
-      <c r="C56" s="60"/>
+      <c r="A56" s="58"/>
+      <c r="B56" s="55"/>
+      <c r="C56" s="72"/>
       <c r="D56" s="13" t="s">
         <v>26</v>
       </c>
@@ -3754,9 +3762,9 @@
       </c>
     </row>
     <row r="57" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="46"/>
-      <c r="B57" s="43"/>
-      <c r="C57" s="60"/>
+      <c r="A57" s="58"/>
+      <c r="B57" s="55"/>
+      <c r="C57" s="72"/>
       <c r="D57" s="13" t="s">
         <v>27</v>
       </c>
@@ -3797,9 +3805,9 @@
       </c>
     </row>
     <row r="58" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="46"/>
-      <c r="B58" s="43"/>
-      <c r="C58" s="60"/>
+      <c r="A58" s="58"/>
+      <c r="B58" s="55"/>
+      <c r="C58" s="72"/>
       <c r="D58" s="13" t="s">
         <v>28</v>
       </c>
@@ -3840,9 +3848,9 @@
       </c>
     </row>
     <row r="59" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="46"/>
-      <c r="B59" s="43"/>
-      <c r="C59" s="60"/>
+      <c r="A59" s="58"/>
+      <c r="B59" s="55"/>
+      <c r="C59" s="72"/>
       <c r="D59" s="13" t="s">
         <v>29</v>
       </c>
@@ -3883,9 +3891,9 @@
       </c>
     </row>
     <row r="60" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A60" s="46"/>
-      <c r="B60" s="43"/>
-      <c r="C60" s="60"/>
+      <c r="A60" s="58"/>
+      <c r="B60" s="55"/>
+      <c r="C60" s="72"/>
       <c r="D60" s="13" t="s">
         <v>30</v>
       </c>
@@ -3926,9 +3934,9 @@
       </c>
     </row>
     <row r="61" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="46"/>
-      <c r="B61" s="43"/>
-      <c r="C61" s="60"/>
+      <c r="A61" s="58"/>
+      <c r="B61" s="55"/>
+      <c r="C61" s="72"/>
       <c r="D61" s="13" t="s">
         <v>31</v>
       </c>
@@ -3969,9 +3977,9 @@
       </c>
     </row>
     <row r="62" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="46"/>
-      <c r="B62" s="43"/>
-      <c r="C62" s="60"/>
+      <c r="A62" s="58"/>
+      <c r="B62" s="55"/>
+      <c r="C62" s="72"/>
       <c r="D62" s="13" t="s">
         <v>32</v>
       </c>
@@ -4012,9 +4020,9 @@
       </c>
     </row>
     <row r="63" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A63" s="46"/>
-      <c r="B63" s="43"/>
-      <c r="C63" s="60"/>
+      <c r="A63" s="58"/>
+      <c r="B63" s="55"/>
+      <c r="C63" s="72"/>
       <c r="D63" s="13" t="s">
         <v>35</v>
       </c>
@@ -4055,9 +4063,9 @@
       </c>
     </row>
     <row r="64" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="46"/>
-      <c r="B64" s="43"/>
-      <c r="C64" s="60"/>
+      <c r="A64" s="58"/>
+      <c r="B64" s="55"/>
+      <c r="C64" s="72"/>
       <c r="D64" s="13" t="s">
         <v>36</v>
       </c>
@@ -4098,9 +4106,9 @@
       </c>
     </row>
     <row r="65" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="46"/>
-      <c r="B65" s="43"/>
-      <c r="C65" s="60"/>
+      <c r="A65" s="58"/>
+      <c r="B65" s="55"/>
+      <c r="C65" s="72"/>
       <c r="D65" s="13" t="s">
         <v>37</v>
       </c>
@@ -4141,9 +4149,9 @@
       </c>
     </row>
     <row r="66" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="46"/>
-      <c r="B66" s="43"/>
-      <c r="C66" s="60"/>
+      <c r="A66" s="58"/>
+      <c r="B66" s="55"/>
+      <c r="C66" s="72"/>
       <c r="D66" s="13" t="s">
         <v>38</v>
       </c>
@@ -4184,9 +4192,9 @@
       </c>
     </row>
     <row r="67" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="46"/>
-      <c r="B67" s="43"/>
-      <c r="C67" s="60"/>
+      <c r="A67" s="58"/>
+      <c r="B67" s="55"/>
+      <c r="C67" s="72"/>
       <c r="D67" s="13" t="s">
         <v>40</v>
       </c>
@@ -4227,9 +4235,9 @@
       </c>
     </row>
     <row r="68" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A68" s="46"/>
-      <c r="B68" s="43"/>
-      <c r="C68" s="61"/>
+      <c r="A68" s="58"/>
+      <c r="B68" s="55"/>
+      <c r="C68" s="73"/>
       <c r="D68" s="13" t="s">
         <v>42</v>
       </c>
@@ -4270,9 +4278,9 @@
       </c>
     </row>
     <row r="69" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="46"/>
-      <c r="B69" s="43"/>
-      <c r="C69" s="39" t="s">
+      <c r="A69" s="58"/>
+      <c r="B69" s="55"/>
+      <c r="C69" s="51" t="s">
         <v>60</v>
       </c>
       <c r="D69" s="14" t="s">
@@ -4315,9 +4323,9 @@
       </c>
     </row>
     <row r="70" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A70" s="46"/>
-      <c r="B70" s="43"/>
-      <c r="C70" s="40"/>
+      <c r="A70" s="58"/>
+      <c r="B70" s="55"/>
+      <c r="C70" s="52"/>
       <c r="D70" s="15" t="s">
         <v>62</v>
       </c>
@@ -4358,9 +4366,9 @@
       </c>
     </row>
     <row r="71" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A71" s="46"/>
-      <c r="B71" s="43"/>
-      <c r="C71" s="40"/>
+      <c r="A71" s="58"/>
+      <c r="B71" s="55"/>
+      <c r="C71" s="52"/>
       <c r="D71" s="15" t="s">
         <v>63</v>
       </c>
@@ -4401,9 +4409,9 @@
       </c>
     </row>
     <row r="72" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="46"/>
-      <c r="B72" s="43"/>
-      <c r="C72" s="40"/>
+      <c r="A72" s="58"/>
+      <c r="B72" s="55"/>
+      <c r="C72" s="52"/>
       <c r="D72" s="15" t="s">
         <v>64</v>
       </c>
@@ -4444,9 +4452,9 @@
       </c>
     </row>
     <row r="73" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A73" s="46"/>
-      <c r="B73" s="43"/>
-      <c r="C73" s="40"/>
+      <c r="A73" s="58"/>
+      <c r="B73" s="55"/>
+      <c r="C73" s="52"/>
       <c r="D73" s="15" t="s">
         <v>65</v>
       </c>
@@ -4487,9 +4495,9 @@
       </c>
     </row>
     <row r="74" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A74" s="46"/>
-      <c r="B74" s="43"/>
-      <c r="C74" s="40"/>
+      <c r="A74" s="58"/>
+      <c r="B74" s="55"/>
+      <c r="C74" s="52"/>
       <c r="D74" s="15" t="s">
         <v>66</v>
       </c>
@@ -4530,9 +4538,9 @@
       </c>
     </row>
     <row r="75" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A75" s="46"/>
-      <c r="B75" s="43"/>
-      <c r="C75" s="40"/>
+      <c r="A75" s="58"/>
+      <c r="B75" s="55"/>
+      <c r="C75" s="52"/>
       <c r="D75" s="15" t="s">
         <v>67</v>
       </c>
@@ -4573,9 +4581,9 @@
       </c>
     </row>
     <row r="76" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="46"/>
-      <c r="B76" s="43"/>
-      <c r="C76" s="40"/>
+      <c r="A76" s="58"/>
+      <c r="B76" s="55"/>
+      <c r="C76" s="52"/>
       <c r="D76" s="15" t="s">
         <v>68</v>
       </c>
@@ -4616,9 +4624,9 @@
       </c>
     </row>
     <row r="77" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="46"/>
-      <c r="B77" s="43"/>
-      <c r="C77" s="40"/>
+      <c r="A77" s="58"/>
+      <c r="B77" s="55"/>
+      <c r="C77" s="52"/>
       <c r="D77" s="15" t="s">
         <v>69</v>
       </c>
@@ -4659,9 +4667,9 @@
       </c>
     </row>
     <row r="78" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A78" s="46"/>
-      <c r="B78" s="43"/>
-      <c r="C78" s="40"/>
+      <c r="A78" s="58"/>
+      <c r="B78" s="55"/>
+      <c r="C78" s="52"/>
       <c r="D78" s="15" t="s">
         <v>70</v>
       </c>
@@ -4702,9 +4710,9 @@
       </c>
     </row>
     <row r="79" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A79" s="46"/>
-      <c r="B79" s="43"/>
-      <c r="C79" s="40"/>
+      <c r="A79" s="58"/>
+      <c r="B79" s="55"/>
+      <c r="C79" s="52"/>
       <c r="D79" s="15" t="s">
         <v>71</v>
       </c>
@@ -4745,9 +4753,9 @@
       </c>
     </row>
     <row r="80" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A80" s="46"/>
-      <c r="B80" s="43"/>
-      <c r="C80" s="40"/>
+      <c r="A80" s="58"/>
+      <c r="B80" s="55"/>
+      <c r="C80" s="52"/>
       <c r="D80" s="15" t="s">
         <v>72</v>
       </c>
@@ -4788,9 +4796,9 @@
       </c>
     </row>
     <row r="81" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A81" s="46"/>
-      <c r="B81" s="43"/>
-      <c r="C81" s="40"/>
+      <c r="A81" s="58"/>
+      <c r="B81" s="55"/>
+      <c r="C81" s="52"/>
       <c r="D81" s="15" t="s">
         <v>73</v>
       </c>
@@ -4831,9 +4839,9 @@
       </c>
     </row>
     <row r="82" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A82" s="46"/>
-      <c r="B82" s="43"/>
-      <c r="C82" s="40"/>
+      <c r="A82" s="58"/>
+      <c r="B82" s="55"/>
+      <c r="C82" s="52"/>
       <c r="D82" s="15" t="s">
         <v>74</v>
       </c>
@@ -4874,9 +4882,9 @@
       </c>
     </row>
     <row r="83" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A83" s="46"/>
-      <c r="B83" s="43"/>
-      <c r="C83" s="40"/>
+      <c r="A83" s="58"/>
+      <c r="B83" s="55"/>
+      <c r="C83" s="52"/>
       <c r="D83" s="15" t="s">
         <v>75</v>
       </c>
@@ -4917,9 +4925,9 @@
       </c>
     </row>
     <row r="84" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A84" s="46"/>
-      <c r="B84" s="43"/>
-      <c r="C84" s="40"/>
+      <c r="A84" s="58"/>
+      <c r="B84" s="55"/>
+      <c r="C84" s="52"/>
       <c r="D84" s="15" t="s">
         <v>76</v>
       </c>
@@ -4960,9 +4968,9 @@
       </c>
     </row>
     <row r="85" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A85" s="46"/>
-      <c r="B85" s="43"/>
-      <c r="C85" s="40"/>
+      <c r="A85" s="58"/>
+      <c r="B85" s="55"/>
+      <c r="C85" s="52"/>
       <c r="D85" s="15" t="s">
         <v>77</v>
       </c>
@@ -5003,9 +5011,9 @@
       </c>
     </row>
     <row r="86" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A86" s="46"/>
-      <c r="B86" s="43"/>
-      <c r="C86" s="40"/>
+      <c r="A86" s="58"/>
+      <c r="B86" s="55"/>
+      <c r="C86" s="52"/>
       <c r="D86" s="15" t="s">
         <v>78</v>
       </c>
@@ -5046,9 +5054,9 @@
       </c>
     </row>
     <row r="87" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A87" s="46"/>
-      <c r="B87" s="43"/>
-      <c r="C87" s="40"/>
+      <c r="A87" s="58"/>
+      <c r="B87" s="55"/>
+      <c r="C87" s="52"/>
       <c r="D87" s="15" t="s">
         <v>79</v>
       </c>
@@ -5089,9 +5097,9 @@
       </c>
     </row>
     <row r="88" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A88" s="46"/>
-      <c r="B88" s="43"/>
-      <c r="C88" s="40"/>
+      <c r="A88" s="58"/>
+      <c r="B88" s="55"/>
+      <c r="C88" s="52"/>
       <c r="D88" s="15" t="s">
         <v>80</v>
       </c>
@@ -5132,9 +5140,9 @@
       </c>
     </row>
     <row r="89" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A89" s="46"/>
-      <c r="B89" s="43"/>
-      <c r="C89" s="40"/>
+      <c r="A89" s="58"/>
+      <c r="B89" s="55"/>
+      <c r="C89" s="52"/>
       <c r="D89" s="15" t="s">
         <v>81</v>
       </c>
@@ -5175,9 +5183,9 @@
       </c>
     </row>
     <row r="90" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A90" s="46"/>
-      <c r="B90" s="43"/>
-      <c r="C90" s="40"/>
+      <c r="A90" s="58"/>
+      <c r="B90" s="55"/>
+      <c r="C90" s="52"/>
       <c r="D90" s="15" t="s">
         <v>82</v>
       </c>
@@ -5218,9 +5226,9 @@
       </c>
     </row>
     <row r="91" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A91" s="46"/>
-      <c r="B91" s="43"/>
-      <c r="C91" s="40"/>
+      <c r="A91" s="58"/>
+      <c r="B91" s="55"/>
+      <c r="C91" s="52"/>
       <c r="D91" s="15" t="s">
         <v>83</v>
       </c>
@@ -5261,9 +5269,9 @@
       </c>
     </row>
     <row r="92" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A92" s="46"/>
-      <c r="B92" s="43"/>
-      <c r="C92" s="40"/>
+      <c r="A92" s="58"/>
+      <c r="B92" s="55"/>
+      <c r="C92" s="52"/>
       <c r="D92" s="15" t="s">
         <v>84</v>
       </c>
@@ -5304,9 +5312,9 @@
       </c>
     </row>
     <row r="93" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A93" s="46"/>
-      <c r="B93" s="43"/>
-      <c r="C93" s="40"/>
+      <c r="A93" s="58"/>
+      <c r="B93" s="55"/>
+      <c r="C93" s="52"/>
       <c r="D93" s="15" t="s">
         <v>85</v>
       </c>
@@ -5347,9 +5355,9 @@
       </c>
     </row>
     <row r="94" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A94" s="46"/>
-      <c r="B94" s="43"/>
-      <c r="C94" s="40"/>
+      <c r="A94" s="58"/>
+      <c r="B94" s="55"/>
+      <c r="C94" s="52"/>
       <c r="D94" s="15" t="s">
         <v>86</v>
       </c>
@@ -5390,9 +5398,9 @@
       </c>
     </row>
     <row r="95" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A95" s="46"/>
-      <c r="B95" s="43"/>
-      <c r="C95" s="40"/>
+      <c r="A95" s="58"/>
+      <c r="B95" s="55"/>
+      <c r="C95" s="52"/>
       <c r="D95" s="16" t="s">
         <v>87</v>
       </c>
@@ -5433,9 +5441,9 @@
       </c>
     </row>
     <row r="96" spans="1:36" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="47"/>
-      <c r="B96" s="44"/>
-      <c r="C96" s="41"/>
+      <c r="A96" s="59"/>
+      <c r="B96" s="56"/>
+      <c r="C96" s="53"/>
       <c r="D96" s="17" t="s">
         <v>88</v>
       </c>
@@ -5611,790 +5619,790 @@
       </c>
     </row>
     <row r="100" spans="1:36" ht="18" x14ac:dyDescent="0.3">
-      <c r="A100" s="68" t="s">
+      <c r="A100" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="B100" s="69"/>
-      <c r="C100" s="69"/>
-      <c r="D100" s="69"/>
-      <c r="E100" s="69"/>
-      <c r="F100" s="69"/>
-      <c r="G100" s="69"/>
-      <c r="H100" s="69"/>
-      <c r="I100" s="69"/>
-      <c r="J100" s="69"/>
-      <c r="K100" s="69"/>
-      <c r="L100" s="69"/>
-      <c r="M100" s="69"/>
-      <c r="N100" s="69"/>
-      <c r="O100" s="69"/>
-      <c r="P100" s="69"/>
-      <c r="Q100" s="69"/>
-      <c r="R100" s="69"/>
-      <c r="S100" s="69"/>
-      <c r="T100" s="69"/>
-      <c r="U100" s="69"/>
-      <c r="V100" s="69"/>
-      <c r="W100" s="69"/>
-      <c r="X100" s="69"/>
-      <c r="Y100" s="69"/>
-      <c r="Z100" s="69"/>
-      <c r="AA100" s="69"/>
-      <c r="AB100" s="69"/>
-      <c r="AC100" s="69"/>
-      <c r="AD100" s="69"/>
-      <c r="AE100" s="69"/>
-      <c r="AF100" s="69"/>
-      <c r="AG100" s="69"/>
-      <c r="AH100" s="69"/>
-      <c r="AI100" s="69"/>
-      <c r="AJ100" s="69"/>
+      <c r="B100" s="50"/>
+      <c r="C100" s="50"/>
+      <c r="D100" s="50"/>
+      <c r="E100" s="50"/>
+      <c r="F100" s="50"/>
+      <c r="G100" s="50"/>
+      <c r="H100" s="50"/>
+      <c r="I100" s="50"/>
+      <c r="J100" s="50"/>
+      <c r="K100" s="50"/>
+      <c r="L100" s="50"/>
+      <c r="M100" s="50"/>
+      <c r="N100" s="50"/>
+      <c r="O100" s="50"/>
+      <c r="P100" s="50"/>
+      <c r="Q100" s="50"/>
+      <c r="R100" s="50"/>
+      <c r="S100" s="50"/>
+      <c r="T100" s="50"/>
+      <c r="U100" s="50"/>
+      <c r="V100" s="50"/>
+      <c r="W100" s="50"/>
+      <c r="X100" s="50"/>
+      <c r="Y100" s="50"/>
+      <c r="Z100" s="50"/>
+      <c r="AA100" s="50"/>
+      <c r="AB100" s="50"/>
+      <c r="AC100" s="50"/>
+      <c r="AD100" s="50"/>
+      <c r="AE100" s="50"/>
+      <c r="AF100" s="50"/>
+      <c r="AG100" s="50"/>
+      <c r="AH100" s="50"/>
+      <c r="AI100" s="50"/>
+      <c r="AJ100" s="50"/>
     </row>
     <row r="101" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A101" s="70"/>
-      <c r="B101" s="71" t="s">
+      <c r="A101" s="39"/>
+      <c r="B101" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="C101" s="72" t="s">
+      <c r="C101" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="D101" s="72" t="s">
-        <v>0</v>
-      </c>
-      <c r="E101" s="73">
+      <c r="D101" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="E101" s="42">
         <v>1</v>
       </c>
-      <c r="F101" s="73">
+      <c r="F101" s="42">
         <v>2</v>
       </c>
-      <c r="G101" s="73">
+      <c r="G101" s="42">
         <v>3</v>
       </c>
-      <c r="H101" s="73">
+      <c r="H101" s="42">
         <v>4</v>
       </c>
-      <c r="I101" s="73">
+      <c r="I101" s="42">
         <v>5</v>
       </c>
-      <c r="J101" s="73">
+      <c r="J101" s="42">
         <v>6</v>
       </c>
-      <c r="K101" s="73">
+      <c r="K101" s="42">
         <v>7</v>
       </c>
-      <c r="L101" s="73">
+      <c r="L101" s="42">
         <v>8</v>
       </c>
-      <c r="M101" s="73">
+      <c r="M101" s="42">
         <v>9</v>
       </c>
-      <c r="N101" s="73">
+      <c r="N101" s="42">
         <v>10</v>
       </c>
-      <c r="O101" s="73">
+      <c r="O101" s="42">
         <v>11</v>
       </c>
-      <c r="P101" s="73">
+      <c r="P101" s="42">
         <v>12</v>
       </c>
-      <c r="Q101" s="73">
+      <c r="Q101" s="42">
         <v>13</v>
       </c>
-      <c r="R101" s="73">
+      <c r="R101" s="42">
         <v>14</v>
       </c>
-      <c r="S101" s="73">
+      <c r="S101" s="42">
         <v>15</v>
       </c>
-      <c r="T101" s="73">
+      <c r="T101" s="42">
         <v>16</v>
       </c>
-      <c r="U101" s="73">
+      <c r="U101" s="42">
         <v>17</v>
       </c>
-      <c r="V101" s="73">
+      <c r="V101" s="42">
         <v>18</v>
       </c>
-      <c r="W101" s="73">
+      <c r="W101" s="42">
         <v>19</v>
       </c>
-      <c r="X101" s="73">
+      <c r="X101" s="42">
         <v>20</v>
       </c>
-      <c r="Y101" s="73">
+      <c r="Y101" s="42">
         <v>21</v>
       </c>
-      <c r="Z101" s="73">
+      <c r="Z101" s="42">
         <v>22</v>
       </c>
-      <c r="AA101" s="73">
+      <c r="AA101" s="42">
         <v>23</v>
       </c>
-      <c r="AB101" s="73">
+      <c r="AB101" s="42">
         <v>24</v>
       </c>
-      <c r="AC101" s="73">
+      <c r="AC101" s="42">
         <v>25</v>
       </c>
-      <c r="AD101" s="73">
+      <c r="AD101" s="42">
         <v>26</v>
       </c>
-      <c r="AE101" s="73">
+      <c r="AE101" s="42">
         <v>27</v>
       </c>
-      <c r="AF101" s="73">
+      <c r="AF101" s="42">
         <v>28</v>
       </c>
-      <c r="AG101" s="73">
+      <c r="AG101" s="42">
         <v>29</v>
       </c>
-      <c r="AH101" s="73">
+      <c r="AH101" s="42">
         <v>30</v>
       </c>
-      <c r="AI101" s="73">
+      <c r="AI101" s="42">
         <v>31</v>
       </c>
-      <c r="AJ101" s="74" t="s">
+      <c r="AJ101" s="43" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A102" s="75"/>
+      <c r="A102" s="44"/>
       <c r="B102" s="36"/>
       <c r="C102" s="36"/>
       <c r="D102" s="35"/>
       <c r="AJ102" s="35"/>
     </row>
     <row r="103" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A103" s="75"/>
+      <c r="A103" s="44"/>
       <c r="B103" s="36"/>
       <c r="C103" s="36"/>
       <c r="D103" s="35"/>
       <c r="AJ103" s="35"/>
     </row>
     <row r="104" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A104" s="75"/>
+      <c r="A104" s="44"/>
       <c r="B104" s="36"/>
       <c r="C104" s="36"/>
       <c r="D104" s="35"/>
       <c r="AJ104" s="36"/>
     </row>
     <row r="105" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A105" s="75"/>
+      <c r="A105" s="44"/>
       <c r="B105" s="36"/>
       <c r="C105" s="36"/>
       <c r="D105" s="35"/>
       <c r="AJ105" s="35"/>
     </row>
     <row r="106" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A106" s="75"/>
+      <c r="A106" s="44"/>
       <c r="B106" s="36"/>
       <c r="C106" s="36"/>
       <c r="D106" s="35"/>
       <c r="AJ106" s="35"/>
     </row>
     <row r="107" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A107" s="75"/>
+      <c r="A107" s="44"/>
       <c r="B107" s="36"/>
       <c r="C107" s="36"/>
       <c r="D107" s="35"/>
       <c r="AJ107" s="35"/>
     </row>
     <row r="108" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A108" s="75"/>
+      <c r="A108" s="44"/>
       <c r="B108" s="36"/>
       <c r="C108" s="36"/>
       <c r="D108" s="35"/>
       <c r="AJ108" s="35"/>
     </row>
     <row r="109" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A109" s="75"/>
+      <c r="A109" s="44"/>
       <c r="B109" s="36"/>
       <c r="C109" s="36"/>
       <c r="D109" s="35"/>
       <c r="AJ109" s="35"/>
     </row>
     <row r="110" spans="1:36" ht="18" x14ac:dyDescent="0.3">
-      <c r="A110" s="68" t="s">
+      <c r="A110" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="B110" s="69"/>
-      <c r="C110" s="69"/>
-      <c r="D110" s="69"/>
-      <c r="E110" s="69"/>
-      <c r="F110" s="69"/>
-      <c r="G110" s="69"/>
-      <c r="H110" s="69"/>
-      <c r="I110" s="69"/>
-      <c r="J110" s="69"/>
-      <c r="K110" s="69"/>
-      <c r="L110" s="69"/>
-      <c r="M110" s="69"/>
-      <c r="N110" s="69"/>
-      <c r="O110" s="69"/>
-      <c r="P110" s="69"/>
-      <c r="Q110" s="69"/>
-      <c r="R110" s="69"/>
-      <c r="S110" s="69"/>
-      <c r="T110" s="69"/>
-      <c r="U110" s="69"/>
-      <c r="V110" s="69"/>
-      <c r="W110" s="69"/>
-      <c r="X110" s="69"/>
-      <c r="Y110" s="69"/>
-      <c r="Z110" s="69"/>
-      <c r="AA110" s="69"/>
-      <c r="AB110" s="69"/>
-      <c r="AC110" s="69"/>
-      <c r="AD110" s="69"/>
-      <c r="AE110" s="69"/>
-      <c r="AF110" s="69"/>
-      <c r="AG110" s="69"/>
-      <c r="AH110" s="69"/>
-      <c r="AI110" s="69"/>
-      <c r="AJ110" s="69"/>
+      <c r="B110" s="50"/>
+      <c r="C110" s="50"/>
+      <c r="D110" s="50"/>
+      <c r="E110" s="50"/>
+      <c r="F110" s="50"/>
+      <c r="G110" s="50"/>
+      <c r="H110" s="50"/>
+      <c r="I110" s="50"/>
+      <c r="J110" s="50"/>
+      <c r="K110" s="50"/>
+      <c r="L110" s="50"/>
+      <c r="M110" s="50"/>
+      <c r="N110" s="50"/>
+      <c r="O110" s="50"/>
+      <c r="P110" s="50"/>
+      <c r="Q110" s="50"/>
+      <c r="R110" s="50"/>
+      <c r="S110" s="50"/>
+      <c r="T110" s="50"/>
+      <c r="U110" s="50"/>
+      <c r="V110" s="50"/>
+      <c r="W110" s="50"/>
+      <c r="X110" s="50"/>
+      <c r="Y110" s="50"/>
+      <c r="Z110" s="50"/>
+      <c r="AA110" s="50"/>
+      <c r="AB110" s="50"/>
+      <c r="AC110" s="50"/>
+      <c r="AD110" s="50"/>
+      <c r="AE110" s="50"/>
+      <c r="AF110" s="50"/>
+      <c r="AG110" s="50"/>
+      <c r="AH110" s="50"/>
+      <c r="AI110" s="50"/>
+      <c r="AJ110" s="50"/>
     </row>
     <row r="111" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A111" s="70"/>
-      <c r="B111" s="71" t="s">
+      <c r="A111" s="39"/>
+      <c r="B111" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="C111" s="72" t="s">
+      <c r="C111" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="D111" s="72" t="s">
-        <v>0</v>
-      </c>
-      <c r="E111" s="73">
+      <c r="D111" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="E111" s="42">
         <v>1</v>
       </c>
-      <c r="F111" s="73">
+      <c r="F111" s="42">
         <v>2</v>
       </c>
-      <c r="G111" s="73">
+      <c r="G111" s="42">
         <v>3</v>
       </c>
-      <c r="H111" s="73">
+      <c r="H111" s="42">
         <v>4</v>
       </c>
-      <c r="I111" s="73">
+      <c r="I111" s="42">
         <v>5</v>
       </c>
-      <c r="J111" s="73">
+      <c r="J111" s="42">
         <v>6</v>
       </c>
-      <c r="K111" s="73">
+      <c r="K111" s="42">
         <v>7</v>
       </c>
-      <c r="L111" s="73">
+      <c r="L111" s="42">
         <v>8</v>
       </c>
-      <c r="M111" s="73">
+      <c r="M111" s="42">
         <v>9</v>
       </c>
-      <c r="N111" s="73">
+      <c r="N111" s="42">
         <v>10</v>
       </c>
-      <c r="O111" s="73">
+      <c r="O111" s="42">
         <v>11</v>
       </c>
-      <c r="P111" s="73">
+      <c r="P111" s="42">
         <v>12</v>
       </c>
-      <c r="Q111" s="73">
+      <c r="Q111" s="42">
         <v>13</v>
       </c>
-      <c r="R111" s="73">
+      <c r="R111" s="42">
         <v>14</v>
       </c>
-      <c r="S111" s="73">
+      <c r="S111" s="42">
         <v>15</v>
       </c>
-      <c r="T111" s="73">
+      <c r="T111" s="42">
         <v>16</v>
       </c>
-      <c r="U111" s="73">
+      <c r="U111" s="42">
         <v>17</v>
       </c>
-      <c r="V111" s="73">
+      <c r="V111" s="42">
         <v>18</v>
       </c>
-      <c r="W111" s="73">
+      <c r="W111" s="42">
         <v>19</v>
       </c>
-      <c r="X111" s="73">
+      <c r="X111" s="42">
         <v>20</v>
       </c>
-      <c r="Y111" s="73">
+      <c r="Y111" s="42">
         <v>21</v>
       </c>
-      <c r="Z111" s="73">
+      <c r="Z111" s="42">
         <v>22</v>
       </c>
-      <c r="AA111" s="73">
+      <c r="AA111" s="42">
         <v>23</v>
       </c>
-      <c r="AB111" s="73">
+      <c r="AB111" s="42">
         <v>24</v>
       </c>
-      <c r="AC111" s="73">
+      <c r="AC111" s="42">
         <v>25</v>
       </c>
-      <c r="AD111" s="73">
+      <c r="AD111" s="42">
         <v>26</v>
       </c>
-      <c r="AE111" s="73">
+      <c r="AE111" s="42">
         <v>27</v>
       </c>
-      <c r="AF111" s="73">
+      <c r="AF111" s="42">
         <v>28</v>
       </c>
-      <c r="AG111" s="73">
+      <c r="AG111" s="42">
         <v>29</v>
       </c>
-      <c r="AH111" s="73">
+      <c r="AH111" s="42">
         <v>30</v>
       </c>
-      <c r="AI111" s="73">
+      <c r="AI111" s="42">
         <v>31</v>
       </c>
-      <c r="AJ111" s="74" t="s">
+      <c r="AJ111" s="43" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="112" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A112" s="75"/>
-      <c r="B112" s="77"/>
-      <c r="C112" s="77"/>
-      <c r="D112" s="75"/>
-      <c r="AJ112" s="75"/>
+      <c r="A112" s="44"/>
+      <c r="B112" s="46"/>
+      <c r="C112" s="46"/>
+      <c r="D112" s="44"/>
+      <c r="AJ112" s="44"/>
     </row>
     <row r="113" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A113" s="75"/>
-      <c r="B113" s="77"/>
-      <c r="C113" s="77"/>
-      <c r="D113" s="75"/>
-      <c r="AJ113" s="75"/>
+      <c r="A113" s="44"/>
+      <c r="B113" s="46"/>
+      <c r="C113" s="46"/>
+      <c r="D113" s="44"/>
+      <c r="AJ113" s="44"/>
     </row>
     <row r="114" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A114" s="75"/>
-      <c r="B114" s="77"/>
-      <c r="C114" s="77"/>
-      <c r="D114" s="75"/>
-      <c r="AJ114" s="75"/>
+      <c r="A114" s="44"/>
+      <c r="B114" s="46"/>
+      <c r="C114" s="46"/>
+      <c r="D114" s="44"/>
+      <c r="AJ114" s="44"/>
     </row>
     <row r="115" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A115" s="75"/>
-      <c r="B115" s="77"/>
-      <c r="C115" s="77"/>
-      <c r="D115" s="75"/>
-      <c r="AJ115" s="75"/>
+      <c r="A115" s="44"/>
+      <c r="B115" s="46"/>
+      <c r="C115" s="46"/>
+      <c r="D115" s="44"/>
+      <c r="AJ115" s="44"/>
     </row>
     <row r="116" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A116" s="75"/>
-      <c r="B116" s="77"/>
-      <c r="C116" s="77"/>
-      <c r="D116" s="75"/>
-      <c r="AJ116" s="75"/>
+      <c r="A116" s="44"/>
+      <c r="B116" s="46"/>
+      <c r="C116" s="46"/>
+      <c r="D116" s="44"/>
+      <c r="AJ116" s="44"/>
     </row>
     <row r="117" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A117" s="75"/>
-      <c r="B117" s="77"/>
-      <c r="C117" s="77"/>
-      <c r="D117" s="75"/>
-      <c r="AJ117" s="75"/>
+      <c r="A117" s="44"/>
+      <c r="B117" s="46"/>
+      <c r="C117" s="46"/>
+      <c r="D117" s="44"/>
+      <c r="AJ117" s="44"/>
     </row>
     <row r="118" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A118" s="75"/>
-      <c r="B118" s="77"/>
-      <c r="C118" s="77"/>
-      <c r="D118" s="75"/>
-      <c r="AJ118" s="75"/>
+      <c r="A118" s="44"/>
+      <c r="B118" s="46"/>
+      <c r="C118" s="46"/>
+      <c r="D118" s="44"/>
+      <c r="AJ118" s="44"/>
     </row>
     <row r="119" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A119" s="75"/>
-      <c r="B119" s="77"/>
-      <c r="C119" s="77"/>
-      <c r="D119" s="75"/>
-      <c r="AJ119" s="75"/>
+      <c r="A119" s="44"/>
+      <c r="B119" s="46"/>
+      <c r="C119" s="46"/>
+      <c r="D119" s="44"/>
+      <c r="AJ119" s="44"/>
     </row>
     <row r="120" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A120" s="75"/>
-      <c r="B120" s="77"/>
-      <c r="C120" s="77"/>
-      <c r="D120" s="75"/>
-      <c r="AJ120" s="75"/>
+      <c r="A120" s="44"/>
+      <c r="B120" s="46"/>
+      <c r="C120" s="46"/>
+      <c r="D120" s="44"/>
+      <c r="AJ120" s="44"/>
     </row>
     <row r="121" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A121" s="75"/>
-      <c r="B121" s="77"/>
-      <c r="C121" s="77"/>
-      <c r="D121" s="75"/>
-      <c r="AJ121" s="75"/>
+      <c r="A121" s="44"/>
+      <c r="B121" s="46"/>
+      <c r="C121" s="46"/>
+      <c r="D121" s="44"/>
+      <c r="AJ121" s="44"/>
     </row>
     <row r="122" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A122" s="75"/>
-      <c r="B122" s="77"/>
-      <c r="C122" s="77"/>
-      <c r="D122" s="75"/>
-      <c r="AJ122" s="75"/>
+      <c r="A122" s="44"/>
+      <c r="B122" s="46"/>
+      <c r="C122" s="46"/>
+      <c r="D122" s="44"/>
+      <c r="AJ122" s="44"/>
     </row>
     <row r="123" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A123" s="75"/>
-      <c r="B123" s="77"/>
-      <c r="C123" s="77"/>
-      <c r="D123" s="75"/>
-      <c r="AJ123" s="75"/>
+      <c r="A123" s="44"/>
+      <c r="B123" s="46"/>
+      <c r="C123" s="46"/>
+      <c r="D123" s="44"/>
+      <c r="AJ123" s="44"/>
     </row>
     <row r="124" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A124" s="75"/>
-      <c r="B124" s="77"/>
-      <c r="C124" s="77"/>
-      <c r="D124" s="75"/>
-      <c r="AJ124" s="75"/>
+      <c r="A124" s="44"/>
+      <c r="B124" s="46"/>
+      <c r="C124" s="46"/>
+      <c r="D124" s="44"/>
+      <c r="AJ124" s="44"/>
     </row>
     <row r="125" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A125" s="75"/>
-      <c r="B125" s="77"/>
-      <c r="C125" s="77"/>
-      <c r="D125" s="75"/>
-      <c r="AJ125" s="75"/>
+      <c r="A125" s="44"/>
+      <c r="B125" s="46"/>
+      <c r="C125" s="46"/>
+      <c r="D125" s="44"/>
+      <c r="AJ125" s="44"/>
     </row>
     <row r="126" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A126" s="75"/>
-      <c r="B126" s="77"/>
-      <c r="C126" s="77"/>
-      <c r="D126" s="75"/>
-      <c r="AJ126" s="75"/>
+      <c r="A126" s="44"/>
+      <c r="B126" s="46"/>
+      <c r="C126" s="46"/>
+      <c r="D126" s="44"/>
+      <c r="AJ126" s="44"/>
     </row>
     <row r="127" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A127" s="75"/>
-      <c r="B127" s="77"/>
-      <c r="C127" s="77"/>
-      <c r="D127" s="75"/>
-      <c r="AJ127" s="75"/>
+      <c r="A127" s="44"/>
+      <c r="B127" s="46"/>
+      <c r="C127" s="46"/>
+      <c r="D127" s="44"/>
+      <c r="AJ127" s="44"/>
     </row>
     <row r="128" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A128" s="75"/>
-      <c r="B128" s="77"/>
-      <c r="C128" s="77"/>
-      <c r="D128" s="75"/>
-      <c r="AJ128" s="75"/>
+      <c r="A128" s="44"/>
+      <c r="B128" s="46"/>
+      <c r="C128" s="46"/>
+      <c r="D128" s="44"/>
+      <c r="AJ128" s="44"/>
     </row>
     <row r="129" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A129" s="75"/>
-      <c r="B129" s="77"/>
-      <c r="C129" s="77"/>
-      <c r="D129" s="75"/>
-      <c r="AJ129" s="75"/>
+      <c r="A129" s="44"/>
+      <c r="B129" s="46"/>
+      <c r="C129" s="46"/>
+      <c r="D129" s="44"/>
+      <c r="AJ129" s="44"/>
     </row>
     <row r="130" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A130" s="75"/>
-      <c r="B130" s="77"/>
-      <c r="C130" s="77"/>
-      <c r="D130" s="75"/>
-      <c r="AJ130" s="75"/>
+      <c r="A130" s="44"/>
+      <c r="B130" s="46"/>
+      <c r="C130" s="46"/>
+      <c r="D130" s="44"/>
+      <c r="AJ130" s="44"/>
     </row>
     <row r="131" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A131" s="75"/>
-      <c r="B131" s="77"/>
-      <c r="C131" s="77"/>
-      <c r="D131" s="75"/>
-      <c r="AJ131" s="75"/>
+      <c r="A131" s="44"/>
+      <c r="B131" s="46"/>
+      <c r="C131" s="46"/>
+      <c r="D131" s="44"/>
+      <c r="AJ131" s="44"/>
     </row>
     <row r="132" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A132" s="75"/>
-      <c r="B132" s="77"/>
-      <c r="C132" s="77"/>
-      <c r="D132" s="75"/>
-      <c r="AJ132" s="75"/>
+      <c r="A132" s="44"/>
+      <c r="B132" s="46"/>
+      <c r="C132" s="46"/>
+      <c r="D132" s="44"/>
+      <c r="AJ132" s="44"/>
     </row>
     <row r="133" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A133" s="75"/>
-      <c r="B133" s="77"/>
-      <c r="C133" s="77"/>
-      <c r="D133" s="75"/>
-      <c r="AJ133" s="75"/>
+      <c r="A133" s="44"/>
+      <c r="B133" s="46"/>
+      <c r="C133" s="46"/>
+      <c r="D133" s="44"/>
+      <c r="AJ133" s="44"/>
     </row>
     <row r="134" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A134" s="75"/>
-      <c r="B134" s="77"/>
-      <c r="C134" s="77"/>
-      <c r="D134" s="75"/>
-      <c r="AJ134" s="75"/>
+      <c r="A134" s="44"/>
+      <c r="B134" s="46"/>
+      <c r="C134" s="46"/>
+      <c r="D134" s="44"/>
+      <c r="AJ134" s="44"/>
     </row>
     <row r="135" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A135" s="75"/>
-      <c r="B135" s="77"/>
-      <c r="C135" s="77"/>
-      <c r="D135" s="75"/>
-      <c r="AJ135" s="75"/>
+      <c r="A135" s="44"/>
+      <c r="B135" s="46"/>
+      <c r="C135" s="46"/>
+      <c r="D135" s="44"/>
+      <c r="AJ135" s="44"/>
     </row>
     <row r="136" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A136" s="75"/>
-      <c r="B136" s="77"/>
-      <c r="C136" s="77"/>
-      <c r="D136" s="75"/>
-      <c r="AJ136" s="75"/>
+      <c r="A136" s="44"/>
+      <c r="B136" s="46"/>
+      <c r="C136" s="46"/>
+      <c r="D136" s="44"/>
+      <c r="AJ136" s="44"/>
     </row>
     <row r="137" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A137" s="75"/>
-      <c r="B137" s="77"/>
-      <c r="C137" s="77"/>
-      <c r="D137" s="75"/>
-      <c r="AJ137" s="75"/>
+      <c r="A137" s="44"/>
+      <c r="B137" s="46"/>
+      <c r="C137" s="46"/>
+      <c r="D137" s="44"/>
+      <c r="AJ137" s="44"/>
     </row>
     <row r="138" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A138" s="75"/>
-      <c r="B138" s="77"/>
-      <c r="C138" s="77"/>
-      <c r="D138" s="75"/>
-      <c r="AJ138" s="75"/>
+      <c r="A138" s="44"/>
+      <c r="B138" s="46"/>
+      <c r="C138" s="46"/>
+      <c r="D138" s="44"/>
+      <c r="AJ138" s="44"/>
     </row>
     <row r="139" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A139" s="75"/>
-      <c r="B139" s="77"/>
-      <c r="C139" s="77"/>
-      <c r="D139" s="75"/>
-      <c r="AJ139" s="75"/>
+      <c r="A139" s="44"/>
+      <c r="B139" s="46"/>
+      <c r="C139" s="46"/>
+      <c r="D139" s="44"/>
+      <c r="AJ139" s="44"/>
     </row>
     <row r="140" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A140" s="75"/>
-      <c r="B140" s="77"/>
-      <c r="C140" s="77"/>
-      <c r="D140" s="75"/>
-      <c r="AJ140" s="75"/>
+      <c r="A140" s="44"/>
+      <c r="B140" s="46"/>
+      <c r="C140" s="46"/>
+      <c r="D140" s="44"/>
+      <c r="AJ140" s="44"/>
     </row>
     <row r="141" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A141" s="75"/>
-      <c r="B141" s="77"/>
-      <c r="C141" s="77"/>
-      <c r="D141" s="75"/>
-      <c r="AJ141" s="75"/>
+      <c r="A141" s="44"/>
+      <c r="B141" s="46"/>
+      <c r="C141" s="46"/>
+      <c r="D141" s="44"/>
+      <c r="AJ141" s="44"/>
     </row>
     <row r="142" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A142" s="75"/>
-      <c r="B142" s="77"/>
-      <c r="C142" s="77"/>
-      <c r="D142" s="75"/>
-      <c r="AJ142" s="75"/>
+      <c r="A142" s="44"/>
+      <c r="B142" s="46"/>
+      <c r="C142" s="46"/>
+      <c r="D142" s="44"/>
+      <c r="AJ142" s="44"/>
     </row>
     <row r="143" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A143" s="75"/>
-      <c r="B143" s="77"/>
-      <c r="C143" s="77"/>
-      <c r="D143" s="75"/>
-      <c r="AJ143" s="75"/>
+      <c r="A143" s="44"/>
+      <c r="B143" s="46"/>
+      <c r="C143" s="46"/>
+      <c r="D143" s="44"/>
+      <c r="AJ143" s="44"/>
     </row>
     <row r="144" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A144" s="75"/>
-      <c r="B144" s="77"/>
-      <c r="C144" s="77"/>
-      <c r="D144" s="75"/>
-      <c r="AJ144" s="75"/>
+      <c r="A144" s="44"/>
+      <c r="B144" s="46"/>
+      <c r="C144" s="46"/>
+      <c r="D144" s="44"/>
+      <c r="AJ144" s="44"/>
     </row>
     <row r="145" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A145" s="75"/>
-      <c r="B145" s="77"/>
-      <c r="C145" s="77"/>
-      <c r="D145" s="75"/>
-      <c r="AJ145" s="75"/>
+      <c r="A145" s="44"/>
+      <c r="B145" s="46"/>
+      <c r="C145" s="46"/>
+      <c r="D145" s="44"/>
+      <c r="AJ145" s="44"/>
     </row>
     <row r="146" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A146" s="75"/>
-      <c r="B146" s="77"/>
-      <c r="C146" s="77"/>
-      <c r="D146" s="75"/>
-      <c r="AJ146" s="75"/>
+      <c r="A146" s="44"/>
+      <c r="B146" s="46"/>
+      <c r="C146" s="46"/>
+      <c r="D146" s="44"/>
+      <c r="AJ146" s="44"/>
     </row>
     <row r="147" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A147" s="75"/>
-      <c r="B147" s="77"/>
-      <c r="C147" s="77"/>
-      <c r="D147" s="75"/>
-      <c r="AJ147" s="75"/>
+      <c r="A147" s="44"/>
+      <c r="B147" s="46"/>
+      <c r="C147" s="46"/>
+      <c r="D147" s="44"/>
+      <c r="AJ147" s="44"/>
     </row>
     <row r="148" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A148" s="75"/>
-      <c r="B148" s="77"/>
-      <c r="C148" s="77"/>
-      <c r="D148" s="75"/>
-      <c r="AJ148" s="75"/>
+      <c r="A148" s="44"/>
+      <c r="B148" s="46"/>
+      <c r="C148" s="46"/>
+      <c r="D148" s="44"/>
+      <c r="AJ148" s="44"/>
     </row>
     <row r="149" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A149" s="75"/>
-      <c r="B149" s="77"/>
-      <c r="C149" s="77"/>
-      <c r="D149" s="75"/>
-      <c r="AJ149" s="75"/>
+      <c r="A149" s="44"/>
+      <c r="B149" s="46"/>
+      <c r="C149" s="46"/>
+      <c r="D149" s="44"/>
+      <c r="AJ149" s="44"/>
     </row>
     <row r="150" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A150" s="75"/>
-      <c r="B150" s="77"/>
-      <c r="C150" s="77"/>
-      <c r="D150" s="75"/>
-      <c r="AJ150" s="75"/>
+      <c r="A150" s="44"/>
+      <c r="B150" s="46"/>
+      <c r="C150" s="46"/>
+      <c r="D150" s="44"/>
+      <c r="AJ150" s="44"/>
     </row>
     <row r="151" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A151" s="75"/>
-      <c r="B151" s="77"/>
-      <c r="C151" s="77"/>
-      <c r="D151" s="75"/>
-      <c r="AJ151" s="75"/>
+      <c r="A151" s="44"/>
+      <c r="B151" s="46"/>
+      <c r="C151" s="46"/>
+      <c r="D151" s="44"/>
+      <c r="AJ151" s="44"/>
     </row>
     <row r="152" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A152" s="75"/>
-      <c r="B152" s="77"/>
-      <c r="C152" s="77"/>
-      <c r="D152" s="75"/>
-      <c r="AJ152" s="75"/>
+      <c r="A152" s="44"/>
+      <c r="B152" s="46"/>
+      <c r="C152" s="46"/>
+      <c r="D152" s="44"/>
+      <c r="AJ152" s="44"/>
     </row>
     <row r="153" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A153" s="75"/>
-      <c r="B153" s="77"/>
-      <c r="C153" s="77"/>
-      <c r="D153" s="75"/>
-      <c r="AJ153" s="75"/>
+      <c r="A153" s="44"/>
+      <c r="B153" s="46"/>
+      <c r="C153" s="46"/>
+      <c r="D153" s="44"/>
+      <c r="AJ153" s="44"/>
     </row>
     <row r="154" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A154" s="75"/>
-      <c r="B154" s="77"/>
-      <c r="C154" s="77"/>
-      <c r="D154" s="75"/>
-      <c r="AJ154" s="75"/>
+      <c r="A154" s="44"/>
+      <c r="B154" s="46"/>
+      <c r="C154" s="46"/>
+      <c r="D154" s="44"/>
+      <c r="AJ154" s="44"/>
     </row>
     <row r="155" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A155" s="75"/>
-      <c r="B155" s="77"/>
-      <c r="C155" s="77"/>
-      <c r="D155" s="75"/>
-      <c r="AJ155" s="75"/>
+      <c r="A155" s="44"/>
+      <c r="B155" s="46"/>
+      <c r="C155" s="46"/>
+      <c r="D155" s="44"/>
+      <c r="AJ155" s="44"/>
     </row>
     <row r="156" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A156" s="75"/>
-      <c r="B156" s="77"/>
-      <c r="C156" s="77"/>
-      <c r="D156" s="75"/>
-      <c r="AJ156" s="75"/>
+      <c r="A156" s="44"/>
+      <c r="B156" s="46"/>
+      <c r="C156" s="46"/>
+      <c r="D156" s="44"/>
+      <c r="AJ156" s="44"/>
     </row>
     <row r="157" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A157" s="75"/>
-      <c r="B157" s="77"/>
-      <c r="C157" s="77"/>
-      <c r="D157" s="75"/>
-      <c r="AJ157" s="75"/>
+      <c r="A157" s="44"/>
+      <c r="B157" s="46"/>
+      <c r="C157" s="46"/>
+      <c r="D157" s="44"/>
+      <c r="AJ157" s="44"/>
     </row>
     <row r="158" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A158" s="75"/>
-      <c r="B158" s="77"/>
-      <c r="C158" s="77"/>
-      <c r="D158" s="75"/>
-      <c r="AJ158" s="75"/>
+      <c r="A158" s="44"/>
+      <c r="B158" s="46"/>
+      <c r="C158" s="46"/>
+      <c r="D158" s="44"/>
+      <c r="AJ158" s="44"/>
     </row>
     <row r="159" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A159" s="75"/>
-      <c r="B159" s="77"/>
-      <c r="C159" s="77"/>
-      <c r="D159" s="75"/>
-      <c r="AJ159" s="75"/>
+      <c r="A159" s="44"/>
+      <c r="B159" s="46"/>
+      <c r="C159" s="46"/>
+      <c r="D159" s="44"/>
+      <c r="AJ159" s="44"/>
     </row>
     <row r="160" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A160" s="75"/>
-      <c r="B160" s="77"/>
-      <c r="C160" s="77"/>
-      <c r="D160" s="75"/>
-      <c r="AJ160" s="75"/>
+      <c r="A160" s="44"/>
+      <c r="B160" s="46"/>
+      <c r="C160" s="46"/>
+      <c r="D160" s="44"/>
+      <c r="AJ160" s="44"/>
     </row>
     <row r="161" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A161" s="75"/>
-      <c r="B161" s="77"/>
-      <c r="C161" s="77"/>
-      <c r="D161" s="75"/>
-      <c r="AJ161" s="75"/>
+      <c r="A161" s="44"/>
+      <c r="B161" s="46"/>
+      <c r="C161" s="46"/>
+      <c r="D161" s="44"/>
+      <c r="AJ161" s="44"/>
     </row>
     <row r="162" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A162" s="75"/>
-      <c r="B162" s="77"/>
-      <c r="C162" s="77"/>
-      <c r="D162" s="75"/>
-      <c r="AJ162" s="75"/>
+      <c r="A162" s="44"/>
+      <c r="B162" s="46"/>
+      <c r="C162" s="46"/>
+      <c r="D162" s="44"/>
+      <c r="AJ162" s="44"/>
     </row>
     <row r="163" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A163" s="75"/>
-      <c r="B163" s="77"/>
-      <c r="C163" s="77"/>
-      <c r="D163" s="75"/>
-      <c r="AJ163" s="75"/>
+      <c r="A163" s="44"/>
+      <c r="B163" s="46"/>
+      <c r="C163" s="46"/>
+      <c r="D163" s="44"/>
+      <c r="AJ163" s="44"/>
     </row>
     <row r="164" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A164" s="75"/>
-      <c r="B164" s="77"/>
-      <c r="C164" s="77"/>
-      <c r="D164" s="75"/>
-      <c r="AJ164" s="75"/>
+      <c r="A164" s="44"/>
+      <c r="B164" s="46"/>
+      <c r="C164" s="46"/>
+      <c r="D164" s="44"/>
+      <c r="AJ164" s="44"/>
     </row>
     <row r="165" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A165" s="75"/>
-      <c r="B165" s="77"/>
-      <c r="C165" s="77"/>
-      <c r="D165" s="75"/>
-      <c r="AJ165" s="75"/>
+      <c r="A165" s="44"/>
+      <c r="B165" s="46"/>
+      <c r="C165" s="46"/>
+      <c r="D165" s="44"/>
+      <c r="AJ165" s="44"/>
     </row>
     <row r="166" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A166" s="75"/>
-      <c r="B166" s="77"/>
-      <c r="C166" s="77"/>
-      <c r="D166" s="75"/>
-      <c r="AJ166" s="75"/>
+      <c r="A166" s="44"/>
+      <c r="B166" s="46"/>
+      <c r="C166" s="46"/>
+      <c r="D166" s="44"/>
+      <c r="AJ166" s="44"/>
     </row>
     <row r="167" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A167" s="75"/>
-      <c r="B167" s="77"/>
-      <c r="C167" s="77"/>
-      <c r="D167" s="75"/>
-      <c r="AJ167" s="75"/>
+      <c r="A167" s="44"/>
+      <c r="B167" s="46"/>
+      <c r="C167" s="46"/>
+      <c r="D167" s="44"/>
+      <c r="AJ167" s="44"/>
     </row>
     <row r="168" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A168" s="75"/>
-      <c r="B168" s="77"/>
-      <c r="C168" s="77"/>
-      <c r="D168" s="75"/>
-      <c r="AJ168" s="75"/>
+      <c r="A168" s="44"/>
+      <c r="B168" s="46"/>
+      <c r="C168" s="46"/>
+      <c r="D168" s="44"/>
+      <c r="AJ168" s="44"/>
     </row>
     <row r="169" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A169" s="75"/>
-      <c r="B169" s="77"/>
-      <c r="C169" s="77"/>
-      <c r="D169" s="75"/>
-      <c r="AJ169" s="75"/>
+      <c r="A169" s="44"/>
+      <c r="B169" s="46"/>
+      <c r="C169" s="46"/>
+      <c r="D169" s="44"/>
+      <c r="AJ169" s="44"/>
     </row>
     <row r="170" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A170" s="75"/>
-      <c r="B170" s="77"/>
-      <c r="C170" s="77"/>
-      <c r="D170" s="75"/>
-      <c r="AJ170" s="75"/>
+      <c r="A170" s="44"/>
+      <c r="B170" s="46"/>
+      <c r="C170" s="46"/>
+      <c r="D170" s="44"/>
+      <c r="AJ170" s="44"/>
     </row>
     <row r="171" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A171" s="75"/>
-      <c r="B171" s="77"/>
-      <c r="C171" s="77"/>
-      <c r="D171" s="75"/>
-      <c r="AJ171" s="75"/>
+      <c r="A171" s="44"/>
+      <c r="B171" s="46"/>
+      <c r="C171" s="46"/>
+      <c r="D171" s="44"/>
+      <c r="AJ171" s="44"/>
     </row>
     <row r="172" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A172" s="75"/>
-      <c r="B172" s="77"/>
-      <c r="C172" s="77"/>
-      <c r="D172" s="75"/>
-      <c r="AJ172" s="75"/>
+      <c r="A172" s="44"/>
+      <c r="B172" s="46"/>
+      <c r="C172" s="46"/>
+      <c r="D172" s="44"/>
+      <c r="AJ172" s="44"/>
     </row>
     <row r="173" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A173" s="75"/>
-      <c r="B173" s="77"/>
-      <c r="C173" s="77"/>
-      <c r="D173" s="75"/>
-      <c r="AJ173" s="75"/>
+      <c r="A173" s="44"/>
+      <c r="B173" s="46"/>
+      <c r="C173" s="46"/>
+      <c r="D173" s="44"/>
+      <c r="AJ173" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -6415,4 +6423,79 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BC75A49-8D2C-4FFE-9273-37761281A792}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.77734375" style="47" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" style="47" customWidth="1"/>
+    <col min="3" max="3" width="24" style="47" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" style="47" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" style="47" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" style="47" customWidth="1"/>
+    <col min="7" max="7" width="35.77734375" style="47" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="48"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E248A85C-13A2-49C6-9ECB-E97C74EC0C40}">
+  <dimension ref="A1:G34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.77734375" style="47" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" style="47" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" style="47" customWidth="1"/>
+    <col min="4" max="4" width="18" style="47" customWidth="1"/>
+    <col min="5" max="5" width="19.77734375" style="47" customWidth="1"/>
+    <col min="6" max="6" width="25.21875" style="47" customWidth="1"/>
+    <col min="7" max="7" width="34.33203125" style="47" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="48"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="48"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="48"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="48"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>